<commit_message>
agregue mejoras en la descarga de retiros
</commit_message>
<xml_diff>
--- a/static/tmp/planificacion3.xlsx
+++ b/static/tmp/planificacion3.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D143"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,13 +459,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>81312</v>
+        <v>81316</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45173.6125</v>
+        <v>45174.6125</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45173.90902777778</v>
+        <v>45174.90902777778</v>
       </c>
     </row>
     <row r="3">
@@ -473,13 +473,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>81804</v>
+        <v>81808</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45173.25</v>
+        <v>45174.25</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45173.57638888889</v>
+        <v>45174.57638888889</v>
       </c>
     </row>
     <row r="4">
@@ -487,13 +487,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>81805</v>
+        <v>81810</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45173.33333333334</v>
+        <v>45174.33333333334</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45173.65972222222</v>
+        <v>45174.65972222222</v>
       </c>
     </row>
     <row r="5">
@@ -501,13 +501,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>81814</v>
+        <v>81811</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45173.41666666666</v>
+        <v>45174.41666666666</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45173.74305555555</v>
+        <v>45174.74305555555</v>
       </c>
     </row>
     <row r="6">
@@ -515,13 +515,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>81820</v>
+        <v>81812</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45173.5</v>
+        <v>45174.5</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45173.82638888889</v>
+        <v>45174.82638888889</v>
       </c>
     </row>
     <row r="7">
@@ -529,13 +529,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>82158</v>
+        <v>82179</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45173.35972222222</v>
+        <v>45174.29166666666</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45173.53819444445</v>
+        <v>45174.70486111111</v>
       </c>
     </row>
     <row r="8">
@@ -543,13 +543,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>82297</v>
+        <v>82281</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45173.43819444445</v>
+        <v>45174.5625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45173.75069444445</v>
+        <v>45174.90486111111</v>
       </c>
     </row>
     <row r="9">
@@ -557,13 +557,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>82336</v>
+        <v>82286</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45173.50555555556</v>
+        <v>45174.58333333334</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45173.85416666666</v>
+        <v>45174.92569444444</v>
       </c>
     </row>
     <row r="10">
@@ -571,13 +571,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>82354</v>
+        <v>82291</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45173.42222222222</v>
+        <v>45174.5</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>45173.72083333333</v>
+        <v>45174.84236111111</v>
       </c>
     </row>
     <row r="11">
@@ -585,13 +585,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>82371</v>
+        <v>82292</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45173.57083333333</v>
+        <v>45174.60416666666</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>45173.86736111111</v>
+        <v>45174.94652777778</v>
       </c>
     </row>
     <row r="12">
@@ -599,13 +599,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>82525</v>
+        <v>82295</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45173.31319444445</v>
+        <v>45174.53125</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>45173.62638888889</v>
+        <v>45174.87361111111</v>
       </c>
     </row>
     <row r="13">
@@ -613,13 +613,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>82595</v>
+        <v>82298</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45173.58333333334</v>
+        <v>45174.31319444445</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>45173.78819444445</v>
+        <v>45174.62569444445</v>
       </c>
     </row>
     <row r="14">
@@ -627,13 +627,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>82636</v>
+        <v>82319</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45173.30138888889</v>
+        <v>45174.41180555556</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>45173.62222222222</v>
+        <v>45174.76041666666</v>
       </c>
     </row>
     <row r="15">
@@ -641,13 +641,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>82643</v>
+        <v>82320</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45173.5</v>
+        <v>45174.55763888889</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>45173.82638888889</v>
+        <v>45174.8625</v>
       </c>
     </row>
     <row r="16">
@@ -655,13 +655,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>82644</v>
+        <v>82321</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45173.36111111111</v>
+        <v>45174.48472222222</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45173.53819444445</v>
+        <v>45174.78333333333</v>
       </c>
     </row>
     <row r="17">
@@ -669,13 +669,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>82647</v>
+        <v>82386</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45173.27777777778</v>
+        <v>45174.30902777778</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>45173.57291666666</v>
+        <v>45174.62638888889</v>
       </c>
     </row>
     <row r="18">
@@ -683,13 +683,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>82675</v>
+        <v>82528</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45173.27083333334</v>
+        <v>45174.43819444445</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>45173.55277777778</v>
+        <v>45174.75138888889</v>
       </c>
     </row>
     <row r="19">
@@ -697,13 +697,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>82676</v>
+        <v>82620</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45173.375</v>
+        <v>45174.37430555555</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>45173.65694444445</v>
+        <v>45174.72986111111</v>
       </c>
     </row>
     <row r="20">
@@ -711,13 +711,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>82677</v>
+        <v>82621</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45173.45763888889</v>
+        <v>45174.41597222222</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>45173.81319444445</v>
+        <v>45174.77152777778</v>
       </c>
     </row>
     <row r="21">
@@ -725,13 +725,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>82685</v>
+        <v>82625</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45173.29166666666</v>
+        <v>45174.27013888889</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>45173.62291666667</v>
+        <v>45174.62569444445</v>
       </c>
     </row>
     <row r="22">
@@ -739,13 +739,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>82713</v>
+        <v>82627</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45173.54097222222</v>
+        <v>45174.29097222222</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>45173.89652777778</v>
+        <v>45174.64652777778</v>
       </c>
     </row>
     <row r="23">
@@ -753,13 +753,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>82719</v>
+        <v>82634</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45173.44791666666</v>
+        <v>45174.33263888889</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45173.65694444445</v>
+        <v>45174.68819444445</v>
       </c>
     </row>
     <row r="24">
@@ -767,13 +767,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>82725</v>
+        <v>82738</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45173.79166666666</v>
+        <v>45174.5</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>45174.14930555555</v>
+        <v>45174.70486111111</v>
       </c>
     </row>
     <row r="25">
@@ -781,13 +781,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>82740</v>
+        <v>82749</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45173.81944444445</v>
+        <v>45174.29166666666</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45173.88888888889</v>
+        <v>45174.62361111111</v>
       </c>
     </row>
     <row r="26">
@@ -795,13 +795,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>82741</v>
+        <v>82959</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45173.84375</v>
+        <v>45174.42569444444</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45173.91319444445</v>
+        <v>45174.77361111111</v>
       </c>
     </row>
     <row r="27">
@@ -809,13 +809,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>82745</v>
+        <v>83082</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45173.31875</v>
+        <v>45174.63888888889</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>45173.49652777778</v>
+        <v>45174.70833333334</v>
       </c>
     </row>
     <row r="28">
@@ -823,13 +823,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>82748</v>
+        <v>83083</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45173.39583333334</v>
+        <v>45174.63888888889</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>45173.72361111111</v>
+        <v>45174.70833333334</v>
       </c>
     </row>
     <row r="29">
@@ -837,13 +837,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>82764</v>
+        <v>83085</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45173.29166666666</v>
+        <v>45174.63888888889</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>45173.69166666667</v>
+        <v>45174.70833333334</v>
       </c>
     </row>
     <row r="30">
@@ -851,13 +851,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>82768</v>
+        <v>83094</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45173.29097222222</v>
+        <v>45174.27083333334</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>45173.64652777778</v>
+        <v>45174.6</v>
       </c>
     </row>
     <row r="31">
@@ -865,13 +865,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>82770</v>
+        <v>83100</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45173.34375</v>
+        <v>45174.54166666666</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>45173.63680555556</v>
+        <v>45174.89930555555</v>
       </c>
     </row>
     <row r="32">
@@ -879,13 +879,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>82797</v>
+        <v>83111</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45173.40486111111</v>
+        <v>45174.66944444444</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>45173.75277777778</v>
+        <v>45174.97638888889</v>
       </c>
     </row>
     <row r="33">
@@ -893,13 +893,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>82947</v>
+        <v>83136</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45173.34236111111</v>
+        <v>45174.33611111111</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>45173.69027777778</v>
+        <v>45174.40555555555</v>
       </c>
     </row>
     <row r="34">
@@ -907,13 +907,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>83021</v>
+        <v>83142</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45173.6875</v>
+        <v>45174.65347222222</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>45174.10069444445</v>
+        <v>45174.95277777778</v>
       </c>
     </row>
     <row r="35">
@@ -921,13 +921,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>83076</v>
+        <v>83147</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45173.33333333334</v>
+        <v>45174.37638888889</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>45173.65486111111</v>
+        <v>45174.44583333333</v>
       </c>
     </row>
     <row r="36">
@@ -935,13 +935,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>83077</v>
+        <v>83156</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45173.33333333334</v>
+        <v>45174.36319444444</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>45173.65486111111</v>
+        <v>45174.53819444445</v>
       </c>
     </row>
     <row r="37">
@@ -949,13 +949,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>83111</v>
+        <v>83160</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45173.66944444444</v>
+        <v>45174.36805555555</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>45173.97638888889</v>
+        <v>45174.4375</v>
       </c>
     </row>
     <row r="38">
@@ -963,13 +963,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>83113</v>
+        <v>83165</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45173.33055555556</v>
+        <v>45174.3625</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>45173.4</v>
+        <v>45174.53819444445</v>
       </c>
     </row>
     <row r="39">
@@ -977,13 +977,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>83120</v>
+        <v>83167</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45173.21458333333</v>
+        <v>45174.38472222222</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>45173.51527777778</v>
+        <v>45174.45416666667</v>
       </c>
     </row>
     <row r="40">
@@ -991,13 +991,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>83124</v>
+        <v>83168</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45173.29166666666</v>
+        <v>45174.56944444445</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>45173.625</v>
+        <v>45174.87083333333</v>
       </c>
     </row>
     <row r="41">
@@ -1005,13 +1005,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>83127</v>
+        <v>83170</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45173.47222222222</v>
+        <v>45174.41388888889</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>45173.54166666666</v>
+        <v>45174.48333333333</v>
       </c>
     </row>
     <row r="42">
@@ -1019,13 +1019,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>83134</v>
+        <v>83181</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45173.41666666666</v>
+        <v>45174.34583333333</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>45173.74236111111</v>
+        <v>45174.41527777778</v>
       </c>
     </row>
     <row r="43">
@@ -1033,13 +1033,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>83135</v>
+        <v>83182</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45173.46041666667</v>
+        <v>45174.57291666666</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>45173.52986111111</v>
+        <v>45174.74652777778</v>
       </c>
     </row>
     <row r="44">
@@ -1047,13 +1047,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>83137</v>
+        <v>83184</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45173.34444444445</v>
+        <v>45174.50902777778</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>45173.41388888889</v>
+        <v>45174.80069444444</v>
       </c>
     </row>
     <row r="45">
@@ -1061,13 +1061,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>83139</v>
+        <v>83185</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45173.36666666667</v>
+        <v>45174.56875</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>45173.43611111111</v>
+        <v>45174.86527777778</v>
       </c>
     </row>
     <row r="46">
@@ -1075,13 +1075,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>83143</v>
+        <v>83186</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45173.47777777778</v>
+        <v>45174.36319444444</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>45173.54722222222</v>
+        <v>45174.65486111111</v>
       </c>
     </row>
     <row r="47">
@@ -1089,13 +1089,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>83145</v>
+        <v>83187</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45173.40208333333</v>
+        <v>45174.33333333334</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>45173.47152777778</v>
+        <v>45174.65486111111</v>
       </c>
     </row>
     <row r="48">
@@ -1103,13 +1103,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>83146</v>
+        <v>83192</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45173.37361111111</v>
+        <v>45174.38055555556</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>45173.44305555556</v>
+        <v>45174.45</v>
       </c>
     </row>
     <row r="49">
@@ -1117,13 +1117,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>83148</v>
+        <v>83198</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45173.47222222222</v>
+        <v>45174.37430555555</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>45173.54166666666</v>
+        <v>45174.44375</v>
       </c>
     </row>
     <row r="50">
@@ -1131,13 +1131,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>83150</v>
+        <v>83203</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45173.44305555556</v>
+        <v>45174.66666666666</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>45173.5125</v>
+        <v>45175.02430555555</v>
       </c>
     </row>
     <row r="51">
@@ -1145,13 +1145,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>83152</v>
+        <v>83205</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45173.4625</v>
+        <v>45174.36597222222</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>45173.53194444445</v>
+        <v>45174.43541666667</v>
       </c>
     </row>
     <row r="52">
@@ -1159,13 +1159,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>83153</v>
+        <v>83210</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>45173.43402777778</v>
+        <v>45174.40763888889</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>45173.50347222222</v>
+        <v>45174.47708333333</v>
       </c>
     </row>
     <row r="53">
@@ -1173,13 +1173,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>83154</v>
+        <v>83214</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>45173.56666666667</v>
+        <v>45174.33055555556</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>45173.63611111111</v>
+        <v>45174.4</v>
       </c>
     </row>
     <row r="54">
@@ -1187,13 +1187,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>83155</v>
+        <v>83215</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>45173.55555555555</v>
+        <v>45174.57152777778</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>45173.625</v>
+        <v>45174.74652777778</v>
       </c>
     </row>
     <row r="55">
@@ -1201,13 +1201,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>83157</v>
+        <v>83217</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>45173.42361111111</v>
+        <v>45174.34236111111</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>45173.49305555555</v>
+        <v>45174.51736111111</v>
       </c>
     </row>
     <row r="56">
@@ -1215,13 +1215,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>83158</v>
+        <v>83219</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>45173.45138888889</v>
+        <v>45174.36180555556</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>45173.52083333334</v>
+        <v>45174.43125</v>
       </c>
     </row>
     <row r="57">
@@ -1229,13 +1229,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>83161</v>
+        <v>83221</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>45173.46805555555</v>
+        <v>45174.5</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>45173.5375</v>
+        <v>45174.82152777778</v>
       </c>
     </row>
     <row r="58">
@@ -1243,13 +1243,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>83163</v>
+        <v>83222</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>45173.59305555555</v>
+        <v>45174.29861111111</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>45173.88263888889</v>
+        <v>45174.6</v>
       </c>
     </row>
     <row r="59">
@@ -1257,13 +1257,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>83164</v>
+        <v>83226</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>45173.33333333334</v>
+        <v>45174.36041666667</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>45173.53819444445</v>
+        <v>45174.53819444445</v>
       </c>
     </row>
     <row r="60">
@@ -1271,13 +1271,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>83169</v>
+        <v>83227</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>45173.40902777778</v>
+        <v>45174.21944444445</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>45173.47847222222</v>
+        <v>45174.39236111111</v>
       </c>
     </row>
     <row r="61">
@@ -1285,13 +1285,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>83173</v>
+        <v>83230</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>45173.48611111111</v>
+        <v>45174.34027777778</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>45173.55555555555</v>
+        <v>45174.40972222222</v>
       </c>
     </row>
     <row r="62">
@@ -1299,13 +1299,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>83174</v>
+        <v>83232</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>45173.40833333333</v>
+        <v>45174.34166666667</v>
       </c>
       <c r="D62" s="2" t="n">
-        <v>45173.47777777778</v>
+        <v>45174.41111111111</v>
       </c>
     </row>
     <row r="63">
@@ -1313,13 +1313,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>83176</v>
+        <v>83257</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>45173.29583333333</v>
+        <v>45174.375</v>
       </c>
       <c r="D63" s="2" t="n">
-        <v>45173.47569444445</v>
+        <v>45174.57986111111</v>
       </c>
     </row>
     <row r="64">
@@ -1327,13 +1327,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>83178</v>
+        <v>83261</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>45173.55277777778</v>
+        <v>45174.33333333334</v>
       </c>
       <c r="D64" s="2" t="n">
-        <v>45173.62222222222</v>
+        <v>45174.53819444445</v>
       </c>
     </row>
     <row r="65">
@@ -1341,13 +1341,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>83179</v>
+        <v>83263</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>45173.43611111111</v>
+        <v>45174.29166666666</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>45173.50555555556</v>
+        <v>45174.49652777778</v>
       </c>
     </row>
     <row r="66">
@@ -1355,13 +1355,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>83180</v>
+        <v>83271</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>45173.38194444445</v>
+        <v>45174.32361111111</v>
       </c>
       <c r="D66" s="2" t="n">
-        <v>45173.45138888889</v>
+        <v>45174.64583333334</v>
       </c>
     </row>
     <row r="67">
@@ -1369,13 +1369,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>83182</v>
+        <v>83272</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45173.57291666666</v>
+        <v>45174.32361111111</v>
       </c>
       <c r="D67" s="2" t="n">
-        <v>45173.74652777778</v>
+        <v>45174.64583333334</v>
       </c>
     </row>
     <row r="68">
@@ -1383,13 +1383,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>83183</v>
+        <v>83273</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45173.40972222222</v>
+        <v>45174.42777777778</v>
       </c>
       <c r="D68" s="2" t="n">
-        <v>45173.47916666666</v>
+        <v>45174.75</v>
       </c>
     </row>
     <row r="69">
@@ -1397,13 +1397,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>83184</v>
+        <v>83274</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>45173.43472222222</v>
+        <v>45174.42777777778</v>
       </c>
       <c r="D69" s="2" t="n">
-        <v>45173.50416666667</v>
+        <v>45174.75</v>
       </c>
     </row>
     <row r="70">
@@ -1411,13 +1411,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>83185</v>
+        <v>83275</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45173.88194444445</v>
+        <v>45174.55277777778</v>
       </c>
       <c r="D70" s="2" t="n">
-        <v>45173.95138888889</v>
+        <v>45174.875</v>
       </c>
     </row>
     <row r="71">
@@ -1425,13 +1425,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>83187</v>
+        <v>83276</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>45173.55972222222</v>
+        <v>45174.55277777778</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>45173.62916666667</v>
+        <v>45174.875</v>
       </c>
     </row>
     <row r="72">
@@ -1439,13 +1439,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>83191</v>
+        <v>83284</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>45173.3125</v>
+        <v>45174.41805555556</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>45173.67013888889</v>
+        <v>45174.72430555556</v>
       </c>
     </row>
     <row r="73">
@@ -1453,13 +1453,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>83195</v>
+        <v>83285</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>45173.55138888889</v>
+        <v>45174.29305555556</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>45173.84513888889</v>
+        <v>45174.59930555556</v>
       </c>
     </row>
     <row r="74">
@@ -1467,13 +1467,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>83196</v>
+        <v>83296</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>45173.55138888889</v>
+        <v>45174.52083333334</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>45173.62083333333</v>
+        <v>45174.70486111111</v>
       </c>
     </row>
     <row r="75">
@@ -1481,13 +1481,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>83199</v>
+        <v>83300</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>45173.83333333334</v>
+        <v>45174.47222222222</v>
       </c>
       <c r="D75" s="2" t="n">
-        <v>45173.90277777778</v>
+        <v>45174.54166666666</v>
       </c>
     </row>
     <row r="76">
@@ -1495,13 +1495,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>83206</v>
+        <v>83306</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>45173.48194444444</v>
+        <v>45174.22916666666</v>
       </c>
       <c r="D76" s="2" t="n">
-        <v>45173.55138888889</v>
+        <v>45174.43402777778</v>
       </c>
     </row>
     <row r="77">
@@ -1509,13 +1509,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>83207</v>
+        <v>83308</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>45173.46111111111</v>
+        <v>45174.3125</v>
       </c>
       <c r="D77" s="2" t="n">
-        <v>45173.53055555555</v>
+        <v>45174.51736111111</v>
       </c>
     </row>
     <row r="78">
@@ -1523,13 +1523,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>83208</v>
+        <v>83348</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>45173.47291666667</v>
+        <v>45174.29166666666</v>
       </c>
       <c r="D78" s="2" t="n">
-        <v>45173.54236111111</v>
+        <v>45174.61944444444</v>
       </c>
     </row>
     <row r="79">
@@ -1537,13 +1537,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>83215</v>
+        <v>83354</v>
       </c>
       <c r="C79" s="2" t="n">
-        <v>45173.89305555556</v>
+        <v>45174.45833333334</v>
       </c>
       <c r="D79" s="2" t="n">
-        <v>45173.9625</v>
+        <v>45174.66319444445</v>
       </c>
     </row>
     <row r="80">
@@ -1551,13 +1551,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>83221</v>
+        <v>83363</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>45173.37916666667</v>
+        <v>45174.5</v>
       </c>
       <c r="D80" s="2" t="n">
-        <v>45173.44861111111</v>
+        <v>45174.83611111111</v>
       </c>
     </row>
     <row r="81">
@@ -1565,13 +1565,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>83222</v>
+        <v>83364</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>45173.47916666666</v>
+        <v>45174.41666666666</v>
       </c>
       <c r="D81" s="2" t="n">
-        <v>45173.54861111111</v>
+        <v>45174.75277777778</v>
       </c>
     </row>
     <row r="82">
@@ -1579,13 +1579,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>83226</v>
+        <v>83375</v>
       </c>
       <c r="C82" s="2" t="n">
-        <v>45173.34861111111</v>
+        <v>45174.41666666666</v>
       </c>
       <c r="D82" s="2" t="n">
-        <v>45173.41805555556</v>
+        <v>45174.82986111111</v>
       </c>
     </row>
     <row r="83">
@@ -1593,13 +1593,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>83233</v>
+        <v>83376</v>
       </c>
       <c r="C83" s="2" t="n">
-        <v>45173.45416666667</v>
+        <v>45174.45833333334</v>
       </c>
       <c r="D83" s="2" t="n">
-        <v>45173.52361111111</v>
+        <v>45174.87152777778</v>
       </c>
     </row>
     <row r="84">
@@ -1607,13 +1607,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>83234</v>
+        <v>83378</v>
       </c>
       <c r="C84" s="2" t="n">
-        <v>45173.38055555556</v>
+        <v>45174.30555555555</v>
       </c>
       <c r="D84" s="2" t="n">
-        <v>45173.45</v>
+        <v>45174.43055555555</v>
       </c>
     </row>
     <row r="85">
@@ -1621,13 +1621,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>83235</v>
+        <v>83386</v>
       </c>
       <c r="C85" s="2" t="n">
-        <v>45173.32152777778</v>
+        <v>45174.48194444444</v>
       </c>
       <c r="D85" s="2" t="n">
-        <v>45173.49652777778</v>
+        <v>45174.55138888889</v>
       </c>
     </row>
     <row r="86">
@@ -1635,13 +1635,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>83237</v>
+        <v>83388</v>
       </c>
       <c r="C86" s="2" t="n">
-        <v>45173.48055555556</v>
+        <v>45174.375</v>
       </c>
       <c r="D86" s="2" t="n">
-        <v>45173.55</v>
+        <v>45174.44444444445</v>
       </c>
     </row>
     <row r="87">
@@ -1649,13 +1649,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>83256</v>
+        <v>83527</v>
       </c>
       <c r="C87" s="2" t="n">
-        <v>45173.375</v>
+        <v>45174.32638888889</v>
       </c>
       <c r="D87" s="2" t="n">
-        <v>45173.57986111111</v>
+        <v>45174.39583333334</v>
       </c>
     </row>
     <row r="88">
@@ -1663,13 +1663,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>83260</v>
+        <v>83530</v>
       </c>
       <c r="C88" s="2" t="n">
-        <v>45173.33333333334</v>
+        <v>45174.34722222222</v>
       </c>
       <c r="D88" s="2" t="n">
-        <v>45173.53819444445</v>
+        <v>45174.41666666666</v>
       </c>
     </row>
     <row r="89">
@@ -1677,13 +1677,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>83262</v>
+        <v>83532</v>
       </c>
       <c r="C89" s="2" t="n">
-        <v>45173.29166666666</v>
+        <v>45174.35416666666</v>
       </c>
       <c r="D89" s="2" t="n">
-        <v>45173.49652777778</v>
+        <v>45174.42361111111</v>
       </c>
     </row>
     <row r="90">
@@ -1691,13 +1691,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>83267</v>
+        <v>83541</v>
       </c>
       <c r="C90" s="2" t="n">
-        <v>45173.32361111111</v>
+        <v>45174.54166666666</v>
       </c>
       <c r="D90" s="2" t="n">
-        <v>45173.64583333334</v>
+        <v>45174.61111111111</v>
       </c>
     </row>
     <row r="91">
@@ -1705,13 +1705,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>83268</v>
+        <v>83547</v>
       </c>
       <c r="C91" s="2" t="n">
-        <v>45173.42777777778</v>
+        <v>45174.44861111111</v>
       </c>
       <c r="D91" s="2" t="n">
-        <v>45173.75</v>
+        <v>45174.51805555556</v>
       </c>
     </row>
     <row r="92">
@@ -1719,13 +1719,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>83269</v>
+        <v>83551</v>
       </c>
       <c r="C92" s="2" t="n">
-        <v>45173.55277777778</v>
+        <v>45174.54305555556</v>
       </c>
       <c r="D92" s="2" t="n">
-        <v>45173.875</v>
+        <v>45174.6125</v>
       </c>
     </row>
     <row r="93">
@@ -1733,13 +1733,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>83270</v>
+        <v>83556</v>
       </c>
       <c r="C93" s="2" t="n">
-        <v>45173.59444444445</v>
+        <v>45174.44513888889</v>
       </c>
       <c r="D93" s="2" t="n">
-        <v>45173.91666666666</v>
+        <v>45174.51458333333</v>
       </c>
     </row>
     <row r="94">
@@ -1747,13 +1747,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>83284</v>
+        <v>83558</v>
       </c>
       <c r="C94" s="2" t="n">
-        <v>45173.87083333333</v>
+        <v>45174.55208333334</v>
       </c>
       <c r="D94" s="2" t="n">
-        <v>45173.94027777778</v>
+        <v>45174.62152777778</v>
       </c>
     </row>
     <row r="95">
@@ -1761,13 +1761,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>83286</v>
+        <v>83562</v>
       </c>
       <c r="C95" s="2" t="n">
-        <v>45173.52222222222</v>
+        <v>45174.47638888889</v>
       </c>
       <c r="D95" s="2" t="n">
-        <v>45173.82847222222</v>
+        <v>45174.54583333333</v>
       </c>
     </row>
     <row r="96">
@@ -1775,13 +1775,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>83296</v>
+        <v>83584</v>
       </c>
       <c r="C96" s="2" t="n">
-        <v>45173.64027777778</v>
+        <v>45174.65694444445</v>
       </c>
       <c r="D96" s="2" t="n">
-        <v>45173.70972222222</v>
+        <v>45174.72638888889</v>
       </c>
     </row>
     <row r="97">
@@ -1789,13 +1789,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>83306</v>
+        <v>83600</v>
       </c>
       <c r="C97" s="2" t="n">
-        <v>45173.41875</v>
+        <v>45174.46041666667</v>
       </c>
       <c r="D97" s="2" t="n">
-        <v>45173.48819444444</v>
+        <v>45174.52986111111</v>
       </c>
     </row>
     <row r="98">
@@ -1803,13 +1803,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>83309</v>
+        <v>83601</v>
       </c>
       <c r="C98" s="2" t="n">
-        <v>45173.35555555556</v>
+        <v>45174.43402777778</v>
       </c>
       <c r="D98" s="2" t="n">
-        <v>45173.425</v>
+        <v>45174.50347222222</v>
       </c>
     </row>
     <row r="99">
@@ -1817,13 +1817,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>83312</v>
+        <v>83602</v>
       </c>
       <c r="C99" s="2" t="n">
-        <v>45173.22916666666</v>
+        <v>45174.47013888889</v>
       </c>
       <c r="D99" s="2" t="n">
-        <v>45173.60347222222</v>
+        <v>45174.53958333333</v>
       </c>
     </row>
     <row r="100">
@@ -1831,13 +1831,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>83313</v>
+        <v>83614</v>
       </c>
       <c r="C100" s="2" t="n">
-        <v>45173.22916666666</v>
+        <v>45174.47777777778</v>
       </c>
       <c r="D100" s="2" t="n">
-        <v>45173.60347222222</v>
+        <v>45174.54722222222</v>
       </c>
     </row>
     <row r="101">
@@ -1845,13 +1845,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>83343</v>
+        <v>83615</v>
       </c>
       <c r="C101" s="2" t="n">
-        <v>45173.34722222222</v>
+        <v>45174.64166666667</v>
       </c>
       <c r="D101" s="2" t="n">
-        <v>45173.41666666666</v>
+        <v>45174.71111111111</v>
       </c>
     </row>
     <row r="102">
@@ -1859,13 +1859,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>83344</v>
+        <v>83617</v>
       </c>
       <c r="C102" s="2" t="n">
-        <v>45173.33611111111</v>
+        <v>45174.42986111111</v>
       </c>
       <c r="D102" s="2" t="n">
-        <v>45173.40555555555</v>
+        <v>45174.49930555555</v>
       </c>
     </row>
     <row r="103">
@@ -1873,13 +1873,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>83345</v>
+        <v>83623</v>
       </c>
       <c r="C103" s="2" t="n">
-        <v>45173.33472222222</v>
+        <v>45174.47916666666</v>
       </c>
       <c r="D103" s="2" t="n">
-        <v>45173.40416666667</v>
+        <v>45174.54861111111</v>
       </c>
     </row>
     <row r="104">
@@ -1887,13 +1887,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>83361</v>
+        <v>83634</v>
       </c>
       <c r="C104" s="2" t="n">
-        <v>45173.33888888889</v>
+        <v>45174.44166666667</v>
       </c>
       <c r="D104" s="2" t="n">
-        <v>45173.40833333333</v>
+        <v>45174.51111111111</v>
       </c>
     </row>
     <row r="105">
@@ -1901,13 +1901,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>83362</v>
+        <v>83646</v>
       </c>
       <c r="C105" s="2" t="n">
-        <v>45173.3375</v>
+        <v>45174.43611111111</v>
       </c>
       <c r="D105" s="2" t="n">
-        <v>45173.40694444445</v>
+        <v>45174.50555555556</v>
       </c>
     </row>
     <row r="106">
@@ -1915,13 +1915,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>83392</v>
+        <v>83650</v>
       </c>
       <c r="C106" s="2" t="n">
-        <v>45173.5</v>
+        <v>45174.33194444444</v>
       </c>
       <c r="D106" s="2" t="n">
-        <v>45173.88402777778</v>
+        <v>45174.40138888889</v>
       </c>
     </row>
     <row r="107">
@@ -1929,13 +1929,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>83393</v>
+        <v>83651</v>
       </c>
       <c r="C107" s="2" t="n">
-        <v>45173.54166666666</v>
+        <v>45174.30763888889</v>
       </c>
       <c r="D107" s="2" t="n">
-        <v>45173.92569444444</v>
+        <v>45174.43263888889</v>
       </c>
     </row>
     <row r="108">
@@ -1943,13 +1943,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>83528</v>
+        <v>83701</v>
       </c>
       <c r="C108" s="2" t="n">
-        <v>45173.88263888889</v>
+        <v>45174.5</v>
       </c>
       <c r="D108" s="2" t="n">
-        <v>45173.95208333333</v>
+        <v>45174.91319444445</v>
       </c>
     </row>
     <row r="109">
@@ -1957,13 +1957,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>83529</v>
+        <v>83702</v>
       </c>
       <c r="C109" s="2" t="n">
-        <v>45173.30972222222</v>
+        <v>45174.25</v>
       </c>
       <c r="D109" s="2" t="n">
-        <v>45173.65625</v>
+        <v>45174.375</v>
       </c>
     </row>
     <row r="110">
@@ -1971,13 +1971,13 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>83536</v>
+        <v>83703</v>
       </c>
       <c r="C110" s="2" t="n">
-        <v>45173.70833333334</v>
+        <v>45174.5</v>
       </c>
       <c r="D110" s="2" t="n">
-        <v>45173.77777777778</v>
+        <v>45174.56944444445</v>
       </c>
     </row>
     <row r="111">
@@ -1985,13 +1985,13 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>83549</v>
+        <v>83728</v>
       </c>
       <c r="C111" s="2" t="n">
-        <v>45173.71111111111</v>
+        <v>45174.49861111111</v>
       </c>
       <c r="D111" s="2" t="n">
-        <v>45173.78055555555</v>
+        <v>45174.56805555556</v>
       </c>
     </row>
     <row r="112">
@@ -1999,13 +1999,13 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>83550</v>
+        <v>83730</v>
       </c>
       <c r="C112" s="2" t="n">
-        <v>45173.85694444444</v>
+        <v>45174.29166666666</v>
       </c>
       <c r="D112" s="2" t="n">
-        <v>45173.92638888889</v>
+        <v>45174.62361111111</v>
       </c>
     </row>
     <row r="113">
@@ -2013,13 +2013,13 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>83552</v>
+        <v>83745</v>
       </c>
       <c r="C113" s="2" t="n">
-        <v>45173.85763888889</v>
+        <v>45174.30138888889</v>
       </c>
       <c r="D113" s="2" t="n">
-        <v>45173.92708333334</v>
+        <v>45174.62152777778</v>
       </c>
     </row>
     <row r="114">
@@ -2027,13 +2027,13 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>83553</v>
+        <v>83748</v>
       </c>
       <c r="C114" s="2" t="n">
-        <v>45173.81597222222</v>
+        <v>45174.70763888889</v>
       </c>
       <c r="D114" s="2" t="n">
-        <v>45173.88541666666</v>
+        <v>45174.77708333333</v>
       </c>
     </row>
     <row r="115">
@@ -2041,13 +2041,13 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>83557</v>
+        <v>83749</v>
       </c>
       <c r="C115" s="2" t="n">
-        <v>45173.86388888889</v>
+        <v>45174.35138888889</v>
       </c>
       <c r="D115" s="2" t="n">
-        <v>45173.93333333333</v>
+        <v>45174.47638888889</v>
       </c>
     </row>
     <row r="116">
@@ -2055,13 +2055,13 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>83559</v>
+        <v>83764</v>
       </c>
       <c r="C116" s="2" t="n">
-        <v>45173.79583333333</v>
+        <v>45174.34722222222</v>
       </c>
       <c r="D116" s="2" t="n">
-        <v>45173.86527777778</v>
+        <v>45174.41666666666</v>
       </c>
     </row>
     <row r="117">
@@ -2069,13 +2069,13 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>83568</v>
+        <v>83786</v>
       </c>
       <c r="C117" s="2" t="n">
-        <v>45173.72777777778</v>
+        <v>45174.34722222222</v>
       </c>
       <c r="D117" s="2" t="n">
-        <v>45173.79722222222</v>
+        <v>45174.62152777778</v>
       </c>
     </row>
     <row r="118">
@@ -2083,13 +2083,13 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>83577</v>
+        <v>83835</v>
       </c>
       <c r="C118" s="2" t="n">
-        <v>45173.88958333333</v>
+        <v>45174.29513888889</v>
       </c>
       <c r="D118" s="2" t="n">
-        <v>45173.95902777778</v>
+        <v>45174.42013888889</v>
       </c>
     </row>
     <row r="119">
@@ -2097,13 +2097,13 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>83578</v>
+        <v>83888</v>
       </c>
       <c r="C119" s="2" t="n">
-        <v>45173.70833333334</v>
+        <v>45174.27083333334</v>
       </c>
       <c r="D119" s="2" t="n">
-        <v>45173.77777777778</v>
+        <v>45174.58680555555</v>
       </c>
     </row>
     <row r="120">
@@ -2111,13 +2111,13 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>83588</v>
+        <v>83895</v>
       </c>
       <c r="C120" s="2" t="n">
-        <v>45173.69722222222</v>
+        <v>45174.41388888889</v>
       </c>
       <c r="D120" s="2" t="n">
-        <v>45173.76666666667</v>
+        <v>45174.57986111111</v>
       </c>
     </row>
     <row r="121">
@@ -2125,13 +2125,13 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>83590</v>
+        <v>83897</v>
       </c>
       <c r="C121" s="2" t="n">
-        <v>45173.73402777778</v>
+        <v>45174.63888888889</v>
       </c>
       <c r="D121" s="2" t="n">
-        <v>45173.80347222222</v>
+        <v>45174.70833333334</v>
       </c>
     </row>
     <row r="122">
@@ -2139,13 +2139,13 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>83611</v>
+        <v>83898</v>
       </c>
       <c r="C122" s="2" t="n">
-        <v>45173.69305555556</v>
+        <v>45174.48472222222</v>
       </c>
       <c r="D122" s="2" t="n">
-        <v>45173.7625</v>
+        <v>45174.55416666667</v>
       </c>
     </row>
     <row r="123">
@@ -2153,13 +2153,13 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>83632</v>
+        <v>83899</v>
       </c>
       <c r="C123" s="2" t="n">
-        <v>45173.68611111111</v>
+        <v>45174.64583333334</v>
       </c>
       <c r="D123" s="2" t="n">
-        <v>45173.75555555556</v>
+        <v>45174.71527777778</v>
       </c>
     </row>
     <row r="124">
@@ -2167,13 +2167,13 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>83649</v>
+        <v>83900</v>
       </c>
       <c r="C124" s="2" t="n">
-        <v>45173.69583333333</v>
+        <v>45174.4375</v>
       </c>
       <c r="D124" s="2" t="n">
-        <v>45173.76527777778</v>
+        <v>45174.50694444445</v>
       </c>
     </row>
     <row r="125">
@@ -2181,13 +2181,13 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>83650</v>
+        <v>83901</v>
       </c>
       <c r="C125" s="2" t="n">
-        <v>45173.81458333333</v>
+        <v>45174.4375</v>
       </c>
       <c r="D125" s="2" t="n">
-        <v>45173.88402777778</v>
+        <v>45174.50694444445</v>
       </c>
     </row>
     <row r="126">
@@ -2195,13 +2195,13 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>83664</v>
+        <v>83902</v>
       </c>
       <c r="C126" s="2" t="n">
-        <v>45173.25</v>
+        <v>45174.4375</v>
       </c>
       <c r="D126" s="2" t="n">
-        <v>45173.57708333333</v>
+        <v>45174.50694444445</v>
       </c>
     </row>
     <row r="127">
@@ -2209,13 +2209,13 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>83691</v>
+        <v>83903</v>
       </c>
       <c r="C127" s="2" t="n">
-        <v>45173.25</v>
+        <v>45174.4375</v>
       </c>
       <c r="D127" s="2" t="n">
-        <v>45173.375</v>
+        <v>45174.50694444445</v>
       </c>
     </row>
     <row r="128">
@@ -2223,13 +2223,13 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>83703</v>
+        <v>83904</v>
       </c>
       <c r="C128" s="2" t="n">
-        <v>45173.33333333334</v>
+        <v>45174.4375</v>
       </c>
       <c r="D128" s="2" t="n">
-        <v>45173.69097222222</v>
+        <v>45174.50694444445</v>
       </c>
     </row>
     <row r="129">
@@ -2237,13 +2237,13 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>83729</v>
+        <v>83905</v>
       </c>
       <c r="C129" s="2" t="n">
-        <v>45173.5</v>
+        <v>45174.4375</v>
       </c>
       <c r="D129" s="2" t="n">
-        <v>45173.82847222222</v>
+        <v>45174.50694444445</v>
       </c>
     </row>
     <row r="130">
@@ -2251,13 +2251,13 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>83730</v>
+        <v>83906</v>
       </c>
       <c r="C130" s="2" t="n">
-        <v>45173.33194444444</v>
+        <v>45174.51388888889</v>
       </c>
       <c r="D130" s="2" t="n">
-        <v>45173.40138888889</v>
+        <v>45174.58333333334</v>
       </c>
     </row>
     <row r="131">
@@ -2265,13 +2265,13 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>83733</v>
+        <v>83907</v>
       </c>
       <c r="C131" s="2" t="n">
-        <v>45173.34444444445</v>
+        <v>45174.51388888889</v>
       </c>
       <c r="D131" s="2" t="n">
-        <v>45173.41388888889</v>
+        <v>45174.58333333334</v>
       </c>
     </row>
     <row r="132">
@@ -2279,13 +2279,13 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>83736</v>
+        <v>83908</v>
       </c>
       <c r="C132" s="2" t="n">
-        <v>45173.70763888889</v>
+        <v>45174.51388888889</v>
       </c>
       <c r="D132" s="2" t="n">
-        <v>45173.77708333333</v>
+        <v>45174.58333333334</v>
       </c>
     </row>
     <row r="133">
@@ -2293,13 +2293,13 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>83752</v>
+        <v>83909</v>
       </c>
       <c r="C133" s="2" t="n">
-        <v>45173.40694444445</v>
+        <v>45174.51388888889</v>
       </c>
       <c r="D133" s="2" t="n">
-        <v>45173.47638888889</v>
+        <v>45174.58333333334</v>
       </c>
     </row>
     <row r="134">
@@ -2307,13 +2307,13 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>83835</v>
+        <v>83910</v>
       </c>
       <c r="C134" s="2" t="n">
-        <v>45173.39166666667</v>
+        <v>45174.5625</v>
       </c>
       <c r="D134" s="2" t="n">
-        <v>45173.46111111111</v>
+        <v>45174.63194444445</v>
       </c>
     </row>
     <row r="135">
@@ -2321,13 +2321,13 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>83836</v>
+        <v>83911</v>
       </c>
       <c r="C135" s="2" t="n">
-        <v>45173.53888888889</v>
+        <v>45174.64583333334</v>
       </c>
       <c r="D135" s="2" t="n">
-        <v>45173.60833333333</v>
+        <v>45174.71527777778</v>
       </c>
     </row>
     <row r="136">
@@ -2335,13 +2335,13 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>83889</v>
+        <v>83912</v>
       </c>
       <c r="C136" s="2" t="n">
-        <v>45173.38611111111</v>
+        <v>45174.64583333334</v>
       </c>
       <c r="D136" s="2" t="n">
-        <v>45173.45555555556</v>
+        <v>45174.71527777778</v>
       </c>
     </row>
     <row r="137">
@@ -2349,13 +2349,13 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>83890</v>
+        <v>83913</v>
       </c>
       <c r="C137" s="2" t="n">
-        <v>45173.40277777778</v>
+        <v>45174.5625</v>
       </c>
       <c r="D137" s="2" t="n">
-        <v>45173.47222222222</v>
+        <v>45174.63194444445</v>
       </c>
     </row>
     <row r="138">
@@ -2363,13 +2363,13 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>83347</v>
+        <v>83914</v>
       </c>
       <c r="C138" s="2" t="n">
-        <v>45173.55138888889</v>
+        <v>45174.5625</v>
       </c>
       <c r="D138" s="2" t="n">
-        <v>45173.62083333333</v>
+        <v>45174.63194444445</v>
       </c>
     </row>
     <row r="139">
@@ -2377,13 +2377,13 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>83346</v>
+        <v>83915</v>
       </c>
       <c r="C139" s="2" t="n">
-        <v>45173.57638888889</v>
+        <v>45174.64583333334</v>
       </c>
       <c r="D139" s="2" t="n">
-        <v>45173.87152777778</v>
+        <v>45174.71527777778</v>
       </c>
     </row>
     <row r="140">
@@ -2391,13 +2391,13 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>83734</v>
+        <v>83916</v>
       </c>
       <c r="C140" s="2" t="n">
-        <v>45173.50416666667</v>
+        <v>45174.5625</v>
       </c>
       <c r="D140" s="2" t="n">
-        <v>45173.62916666667</v>
+        <v>45174.63194444445</v>
       </c>
     </row>
     <row r="141">
@@ -2405,13 +2405,13 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>83732</v>
+        <v>83917</v>
       </c>
       <c r="C141" s="2" t="n">
-        <v>45173.60416666666</v>
+        <v>45174.5625</v>
       </c>
       <c r="D141" s="2" t="n">
-        <v>45173.72916666666</v>
+        <v>45174.63194444445</v>
       </c>
     </row>
     <row r="142">
@@ -2419,13 +2419,13 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>83735</v>
+        <v>83918</v>
       </c>
       <c r="C142" s="2" t="n">
-        <v>45173.86666666667</v>
+        <v>45174.64583333334</v>
       </c>
       <c r="D142" s="2" t="n">
-        <v>45173.93611111111</v>
+        <v>45174.71527777778</v>
       </c>
     </row>
     <row r="143">
@@ -2433,13 +2433,41 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>83731</v>
+        <v>83919</v>
       </c>
       <c r="C143" s="2" t="n">
-        <v>45173.47916666666</v>
+        <v>45174.5625</v>
       </c>
       <c r="D143" s="2" t="n">
-        <v>45173.54861111111</v>
+        <v>45174.63194444445</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>83603</v>
+      </c>
+      <c r="C144" s="2" t="n">
+        <v>45174.5625</v>
+      </c>
+      <c r="D144" s="2" t="n">
+        <v>45174.63194444445</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>83581</v>
+      </c>
+      <c r="C145" s="2" t="n">
+        <v>45174.64583333334</v>
+      </c>
+      <c r="D145" s="2" t="n">
+        <v>45174.71527777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificaciones en carta gantt
</commit_message>
<xml_diff>
--- a/static/tmp/planificacion3.xlsx
+++ b/static/tmp/planificacion3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>id</t>
   </si>
@@ -28,742 +28,712 @@
     <t>DT final</t>
   </si>
   <si>
-    <t>(90528, 0    90528-p
-1    90528-p
-2    90528-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(97713, 3    97713-p
-4    97713-p
-5    97713-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99087, 6    99087-p
-7    99087-p
-8    99087-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99088, 9     99088-p
-10    99088-p
-11    99088-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99089, 12    99089-p
-13    99089-p
-14    99089-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99141, 15    99141-p
-16    99141-p
-17    99141-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99143, 18    99143-p
-19    99143-p
-20    99143-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99698, 21    99698-p
-22    99698-p
-23    99698-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99700, 24    99700-p
-25    99700-p
-26    99700-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99702, 27    99702-p
-28    99702-p
-29    99702-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99706, 30    99706-p
-31    99706-p
-32    99706-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99711, 33    99711-p
-34    99711-p
-35    99711-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99713, 36    99713-p
-37    99713-p
-38    99713-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99751, 39    99751-p
-40    99751-p
-41    99751-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99756, 42    99756-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99803, 43    99803-p
-44    99803-p
-45    99803-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99824, 46    99824-p
-47    99824-p
-48    99824-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99854, 49    99854-p
-50    99854-p
-51    99854-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99907, 52    99907-p
+    <t>(99138, 0    99138-p
+1    99138-p
+2    99138-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99139, 3    99139-p
+4    99139-p
+5    99139-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99140, 6    99140-p
+7    99140-p
+8    99140-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99145, 9     99145-p
+10    99145-p
+11    99145-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99487, 12    99487-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99647, 13    99647-p
+14    99647-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99696, 15    99696-p
+16    99696-p
+17    99696-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99699, 18    99699-p
+19    99699-p
+20    99699-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99701, 21    99701-p
+22    99701-p
+23    99701-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99704, 24    99704-p
+25    99704-p
+26    99704-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99709, 27    99709-p
+28    99709-p
+29    99709-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99772, 30    99772-p
+31    99772-p
+32    99772-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99812, 33    99812-p
+34    99812-p
+35    99812-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99813, 36    99813-p
+37    99813-p
+38    99813-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99839, 39    99839-p
+40    99839-p
+41    99839-p
+42    99839-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99843, 43    99843-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99854, 44    99854-p
+45    99854-p
+46    99854-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99869, 47    99869-p
+48    99869-p
+49    99869-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99871, 50    99871-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99907, 51    99907-p
+52    99907-p
 53    99907-p
-54    99907-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99944, 55    99944-p
-56    99944-p
-57    99944-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99945, 58    99945-p
-59    99945-p
-60    99945-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99965, 61    99965-p
-62    99965-p
-63    99965-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99968, 64    99968-p
-65    99968-p
-66    99968-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99973, 67    99973-p
-68    99973-p
-69    99973-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(99997, 70    99997-p
-71    99997-p
-72    99997-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100006, 73    100006-p
-74    100006-p
-75    100006-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100019, 76    100019-p
-77    100019-p
-78    100019-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100035, 79    100035-p
-80    100035-p
-81    100035-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100043, 82    100043-p
-83    100043-p
-84    100043-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100058, 85    100058-p
-86    100058-p
-87    100058-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100069, 88    100069-p
-89    100069-p
-90    100069-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100070, 91    100070-p
-92    100070-p
-93    100070-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100074, 94    100074-p
-95    100074-p
-96    100074-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100077, 97    100077-p
-98    100077-p
-99    100077-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100092, 100    100092-p
-101    100092-p
-102    100092-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100134, 103    100134-p
-104    100134-p
-105    100134-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100142, 106    100142-p
-107    100142-p
-108    100142-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100261, 109    100261-p
-110    100261-p
-111    100261-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100262, 112    100262-p
-113    100262-p
-114    100262-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100263, 115    100263-p
-116    100263-p
-117    100263-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100264, 118    100264-p
-119    100264-p
-120    100264-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100284, 121    100284-p
-122    100284-p
-123    100284-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100289, 124    100289-p
-125    100289-p
-126    100289-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100326, 127    100326-p
-128    100326-p
-129    100326-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100327, 130    100327-p
-131    100327-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100331, 132    100331-p
-133    100331-p
-134    100331-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100335, 135    100335-p
-136    100335-p
-137    100335-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100341, 138    100341-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100362, 139    100362-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100363, 140    100363-p
-141    100363-p
-142    100363-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100364, 143    100364-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100373, 144    100373-p
-145    100373-p
-146    100373-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100379, 147    100379-p
-148    100379-p
-149    100379-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100382, 150    100382-p
-151    100382-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100386, 152    100386-p
-153    100386-p
-154    100386-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100388, 155    100388-p
-156    100388-p
-157    100388-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100402, 158    100402-p
-159    100402-p
-160    100402-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100417, 161    100417-p
-162    100417-p
-163    100417-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100421, 164    100421-p
-165    100421-p
-166    100421-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100434, 167    100434-p
-168    100434-p
-169    100434-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100442, 170    100442-p
-171    100442-p
-172    100442-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100444, 173    100444-p
-174    100444-p
-175    100444-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100465, 176    100465-p
-177    100465-p
-178    100465-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100477, 179    100477-p
-180    100477-p
-181    100477-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100479, 182    100479-p
-183    100479-p
-184    100479-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100490, 185    100490-p
-186    100490-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100496, 187    100496-p
-188    100496-p
-189    100496-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100511, 190    100511-p
-191    100511-p
-192    100511-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100530, 193    100530-p
-194    100530-p
-195    100530-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100540, 196    100540-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100541, 197    100541-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100542, 198    100542-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100543, 199    100543-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100553, 200    100553-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100554, 201    100554-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100556, 202    100556-p
-203    100556-p
-204    100556-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100590, 205    100590-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100603, 206    100603-p
-207    100603-p
-208    100603-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100604, 209    100604-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100610, 210    100610-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100611, 211    100611-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100612, 212    100612-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100613, 213    100613-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100614, 214    100614-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100615, 215    100615-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100616, 216    100616-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100617, 217    100617-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100631, 312    100631-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100636, 218    100636-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100640, 306    100640-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100642, 219    100642-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100650, 220    100650-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100651, 221    100651-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100653, 222    100653-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100654, 223    100654-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100656, 224    100656-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100658, 225    100658-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100660, 226    100660-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100661, 227    100661-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100663, 228    100663-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100667, 229    100667-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100669, 230    100669-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100672, 231    100672-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100673, 232    100673-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100674, 233    100674-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100678, 234    100678-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100680, 235    100680-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100681, 236    100681-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100682, 237    100682-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100684, 238    100684-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100685, 239    100685-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100686, 240    100686-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100689, 241    100689-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100690, 242    100690-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100695, 243    100695-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100696, 244    100696-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100702, 245    100702-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100703, 329    100703-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100706, 246    100706-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100707, 247    100707-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100710, 248    100710-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100728, 249    100728-p
-250    100728-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100729, 251    100729-p
-252    100729-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100734, 253    100734-p
-254    100734-p
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100736, 255    100736-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100738, 256    100738-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100739, 257    100739-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100740, 258    100740-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100753, 259    100753-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100766, 260    100766-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100767, 261    100767-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100768, 262    100768-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100770, 263    100770-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100771, 264    100771-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100772, 265    100772-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100773, 266    100773-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100774, 267    100774-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100775, 268    100775-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100778, 269    100778-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100782, 270    100782-r
-340    100782-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100794, 271    100794-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100795, 272    100795-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100796, 273    100796-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100797, 274    100797-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100801, 275    100801-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100802, 276    100802-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100803, 277    100803-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100804, 278    100804-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100805, 279    100805-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100807, 287    100807-r
-Name: id_modelo, dtype: object)</t>
-  </si>
-  <si>
-    <t>(100821, 280    100821-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99947, 54    99947-p
+55    99947-p
+56    99947-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99976, 57    99976-p
+58    99976-p
+59    99976-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99994, 60    99994-p
+61    99994-p
+62    99994-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(99997, 63    99997-p
+64    99997-p
+65    99997-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100024, 66    100024-p
+67    100024-p
+68    100024-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100031, 69    100031-p
+70    100031-p
+71    100031-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100035, 72    100035-p
+73    100035-p
+74    100035-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100041, 75    100041-p
+76    100041-p
+77    100041-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100043, 78    100043-p
+79    100043-p
+80    100043-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100050, 81    100050-p
+82    100050-p
+83    100050-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100053, 84    100053-p
+85    100053-p
+86    100053-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100054, 87    100054-p
+88    100054-p
+89    100054-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100060, 90    100060-p
+91    100060-p
+92    100060-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100061, 93    100061-p
+94    100061-p
+95    100061-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100068, 96    100068-p
+97    100068-p
+98    100068-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100074, 99     100074-p
+100    100074-p
+101    100074-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100076, 102    100076-p
+103    100076-p
+104    100076-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100091, 105    100091-p
+106    100091-p
+107    100091-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100092, 108    100092-p
+109    100092-p
+110    100092-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100097, 111    100097-p
+112    100097-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100115, 113    100115-p
+114    100115-p
+115    100115-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100127, 116    100127-p
+117    100127-p
+118    100127-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100135, 119    100135-p
+120    100135-p
+121    100135-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100277, 122    100277-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100278, 123    100278-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100285, 124    100285-p
+125    100285-p
+126    100285-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100288, 127    100288-p
+128    100288-p
+129    100288-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100290, 130    100290-p
+131    100290-p
+132    100290-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100329, 133    100329-p
+134    100329-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100332, 135    100332-p
+136    100332-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100343, 137    100343-p
+138    100343-p
+139    100343-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100351, 140    100351-p
+141    100351-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100356, 142    100356-p
+143    100356-p
+144    100356-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100362, 145    100362-p
+146    100362-p
+147    100362-p
+148    100362-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100390, 149    100390-p
+150    100390-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100401, 151    100401-p
+152    100401-p
+153    100401-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100402, 154    100402-p
+155    100402-p
+156    100402-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100406, 157    100406-p
+158    100406-p
+159    100406-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100408, 160    100408-p
+161    100408-p
+162    100408-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100409, 163    100409-p
+164    100409-p
+165    100409-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100420, 166    100420-p
+167    100420-p
+168    100420-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100421, 169    100421-p
+170    100421-p
+171    100421-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100422, 172    100422-p
+173    100422-p
+174    100422-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100423, 175    100423-p
+176    100423-p
+177    100423-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100425, 178    100425-p
+179    100425-p
+180    100425-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100441, 181    100441-p
+182    100441-p
+183    100441-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100444, 184    100444-p
+185    100444-p
+186    100444-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100456, 187    100456-p
+188    100456-p
+189    100456-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100465, 190    100465-p
+191    100465-p
+192    100465-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100467, 193    100467-p
+194    100467-p
+195    100467-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100475, 196    100475-p
+197    100475-p
+198    100475-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100477, 199    100477-p
+200    100477-p
+201    100477-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100479, 202    100479-p
+203    100479-p
+204    100479-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100484, 205    100484-p
+206    100484-p
+207    100484-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100490, 208    100490-p
+209    100490-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100503, 210    100503-p
+211    100503-p
+212    100503-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100511, 213    100511-p
+214    100511-p
+215    100511-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100541, 216    100541-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100542, 217    100542-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100543, 218    100543-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100546, 219    100546-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100553, 220    100553-p
+221    100553-r
+222    100553-p
+223    100553-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100554, 224    100554-p
+225    100554-p
+226    100554-p
+227    100554-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100590, 228    100590-p
+229    100590-r
+230    100590-p
+231    100590-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100604, 232    100604-p
+233    100604-p
+234    100604-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100605, 235    100605-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100606, 236    100606-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100614, 237    100614-p
+238    100614-p
+239    100614-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100618, 240    100618-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100619, 241    100619-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100620, 242    100620-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100621, 243    100621-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100622, 244    100622-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100623, 245    100623-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100624, 246    100624-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100625, 247    100625-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100628, 248    100628-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100629, 249    100629-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100630, 250    100630-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100632, 251    100632-r
+252    100632-p
+253    100632-p
+254    100632-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100643, 255    100643-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100644, 256    100644-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100645, 257    100645-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100646, 258    100646-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100654, 259    100654-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100656, 260    100656-p
+261    100656-p
+262    100656-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100660, 263    100660-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100672, 264    100672-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100674, 265    100674-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100678, 266    100678-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100710, 267    100710-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100736, 268    100736-p
+269    100736-p
+270    100736-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100738, 271    100738-p
+272    100738-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100739, 273    100739-p
+274    100739-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100740, 275    100740-p
+276    100740-p
+277    100740-p
+278    100740-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100741, 279    100741-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100749, 280    100749-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100750, 281    100750-p
+282    100750-p
+283    100750-p
+284    100750-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100752, 285    100752-r
+286    100752-p
+287    100752-p
+288    100752-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100753, 289    100753-p
+290    100753-p
+291    100753-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100776, 292    100776-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100777, 293    100777-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100782, 294    100782-r
+317    100782-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100800, 295    100800-r
+296    100800-p
+297    100800-p
+298    100800-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100801, 299    100801-p
+300    100801-p
+301    100801-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100804, 302    100804-p
+303    100804-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100821, 304    100821-p
+305    100821-p
+306    100821-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100860, 307    100860-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100862, 308    100862-r
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100904, 309    100904-p
+310    100904-p
+Name: id_modelo, dtype: object)</t>
+  </si>
+  <si>
+    <t>(100905, 311    100905-p
+312    100905-p
+313    100905-p
+314    100905-r
 Name: id_modelo, dtype: object)</t>
   </si>
 </sst>
@@ -1126,7 +1096,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1151,16 +1121,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>90528</v>
+        <v>99138</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2">
-        <v>45448.41666666666</v>
+        <v>45449.27986111111</v>
       </c>
       <c r="E2" s="2">
-        <v>45448.77777777778</v>
+        <v>45449.53788888889</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1168,16 +1138,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>97713</v>
+        <v>99139</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2">
-        <v>45448.41666666666</v>
+        <v>45449.27986111111</v>
       </c>
       <c r="E3" s="2">
-        <v>45448.74183333333</v>
+        <v>45449.53788888889</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1185,16 +1155,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>99087</v>
+        <v>99140</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>45448.29166666666</v>
+        <v>45449.31111111111</v>
       </c>
       <c r="E4" s="2">
-        <v>45448.61683333333</v>
+        <v>45449.56913888889</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1202,16 +1172,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>99088</v>
+        <v>99145</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>45448.33333333334</v>
+        <v>45449.44652777778</v>
       </c>
       <c r="E5" s="2">
-        <v>45448.6585</v>
+        <v>45449.70455555555</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1219,16 +1189,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>99089</v>
+        <v>99487</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2">
-        <v>45448.375</v>
+        <v>45448.84722222222</v>
       </c>
       <c r="E6" s="2">
-        <v>45448.70016666667</v>
+        <v>45448.90277777778</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1236,16 +1206,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>99141</v>
+        <v>99647</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2">
-        <v>45448.31111111111</v>
+        <v>45449.25</v>
       </c>
       <c r="E7" s="2">
-        <v>45448.56913888889</v>
+        <v>45449.44130555556</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1253,16 +1223,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>99143</v>
+        <v>99696</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="2">
-        <v>45448.34236111111</v>
+        <v>45449.36319444444</v>
       </c>
       <c r="E8" s="2">
-        <v>45448.60038888889</v>
+        <v>45449.62122222222</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1270,16 +1240,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>99698</v>
+        <v>99699</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="2">
-        <v>45448.45694444444</v>
+        <v>45449.44652777778</v>
       </c>
       <c r="E9" s="2">
-        <v>45448.71497222222</v>
+        <v>45449.70455555555</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1287,16 +1257,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>99700</v>
+        <v>99701</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2">
-        <v>45448.61319444444</v>
+        <v>45449.61319444444</v>
       </c>
       <c r="E10" s="2">
-        <v>45448.87122222222</v>
+        <v>45449.87122222222</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1304,16 +1274,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>99702</v>
+        <v>99704</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2">
-        <v>45448.58194444444</v>
+        <v>45449.55069444444</v>
       </c>
       <c r="E11" s="2">
-        <v>45448.83997222222</v>
+        <v>45449.80872222222</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1321,16 +1291,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>99706</v>
+        <v>99709</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2">
-        <v>45448.42569444444</v>
+        <v>45449.58194444444</v>
       </c>
       <c r="E12" s="2">
-        <v>45448.68372222222</v>
+        <v>45449.83997222222</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1338,16 +1308,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>99711</v>
+        <v>99772</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2">
-        <v>45448.55069444444</v>
+        <v>45449.47777777778</v>
       </c>
       <c r="E13" s="2">
-        <v>45448.80872222222</v>
+        <v>45449.73580555555</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1355,16 +1325,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>99713</v>
+        <v>99812</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2">
-        <v>45448.27986111111</v>
+        <v>45449.28680555556</v>
       </c>
       <c r="E14" s="2">
-        <v>45448.53788888889</v>
+        <v>45449.55809722222</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1372,16 +1342,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>99751</v>
+        <v>99813</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="2">
-        <v>45448.5</v>
+        <v>45449.28680555556</v>
       </c>
       <c r="E15" s="2">
-        <v>45448.86111111111</v>
+        <v>45449.55809722222</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1389,16 +1359,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>99756</v>
+        <v>99839</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2">
-        <v>45448.52708333333</v>
+        <v>45448.72222222222</v>
       </c>
       <c r="E16" s="2">
-        <v>45448.58263888889</v>
+        <v>45449.87708333333</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1406,16 +1376,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>99803</v>
+        <v>99843</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="2">
-        <v>45448.32013888889</v>
+        <v>45448.72916666666</v>
       </c>
       <c r="E17" s="2">
-        <v>45448.55138888889</v>
+        <v>45448.78472222222</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1423,16 +1393,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>99824</v>
+        <v>99854</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="2">
-        <v>45448.32152777778</v>
+        <v>45448.70833333334</v>
       </c>
       <c r="E18" s="2">
-        <v>45448.57488888889</v>
+        <v>45448.975</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1440,16 +1410,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>99854</v>
+        <v>99869</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="2">
-        <v>45448.70833333334</v>
+        <v>45448.94930555556</v>
       </c>
       <c r="E19" s="2">
-        <v>45448.975</v>
+        <v>45449.20972222222</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1457,16 +1427,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>99907</v>
+        <v>99871</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="2">
-        <v>45448.6875</v>
+        <v>45448.83194444444</v>
       </c>
       <c r="E20" s="2">
-        <v>45448.98631944445</v>
+        <v>45448.8875</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1474,16 +1444,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>99944</v>
+        <v>99907</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="2">
-        <v>45448.61736111111</v>
+        <v>45448.6875</v>
       </c>
       <c r="E21" s="2">
-        <v>45448.91180555556</v>
+        <v>45448.98631944445</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1491,16 +1461,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>99945</v>
+        <v>99947</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="2">
-        <v>45448.54166666666</v>
+        <v>45449.61041666667</v>
       </c>
       <c r="E22" s="2">
-        <v>45448.87777777778</v>
+        <v>45449.94444444445</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1508,16 +1478,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>99965</v>
+        <v>99976</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="2">
-        <v>45448.31041666667</v>
+        <v>45449.35416666666</v>
       </c>
       <c r="E23" s="2">
-        <v>45448.54722222222</v>
+        <v>45449.69444444445</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1525,16 +1495,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>99968</v>
+        <v>99994</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="2">
-        <v>45448.47708333333</v>
+        <v>45449.66666666666</v>
       </c>
       <c r="E24" s="2">
-        <v>45448.71388888889</v>
+        <v>45450.02777777778</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1542,16 +1512,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>99973</v>
+        <v>99997</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="2">
-        <v>45448.625</v>
+        <v>45448.69722222222</v>
       </c>
       <c r="E25" s="2">
-        <v>45448.9625</v>
+        <v>45448.96865277778</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1559,16 +1529,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>99997</v>
+        <v>100024</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="2">
-        <v>45448.69722222222</v>
+        <v>45449.6</v>
       </c>
       <c r="E26" s="2">
-        <v>45448.96865277778</v>
+        <v>45449.97936111111</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1576,16 +1546,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>100006</v>
+        <v>100031</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="2">
-        <v>45448.47569444445</v>
+        <v>45449.1875</v>
       </c>
       <c r="E27" s="2">
-        <v>45448.80972222222</v>
+        <v>45449.56263888889</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1593,16 +1563,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>100019</v>
+        <v>100035</v>
       </c>
       <c r="C28" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="2">
-        <v>45448.5625</v>
+        <v>45448.66666666666</v>
       </c>
       <c r="E28" s="2">
-        <v>45448.90008333333</v>
+        <v>45449.08333333334</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1610,16 +1580,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>100035</v>
+        <v>100041</v>
       </c>
       <c r="C29" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="2">
-        <v>45448.66666666666</v>
+        <v>45448.6875</v>
       </c>
       <c r="E29" s="2">
-        <v>45449.08333333334</v>
+        <v>45449.10416666666</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1644,16 +1614,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>100058</v>
+        <v>100050</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="2">
-        <v>45448.27083333334</v>
+        <v>45449.54166666666</v>
       </c>
       <c r="E31" s="2">
-        <v>45448.6875</v>
+        <v>45449.86866666667</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1661,16 +1631,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>100069</v>
+        <v>100053</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="2">
-        <v>45448.35416666666</v>
+        <v>45449.33333333334</v>
       </c>
       <c r="E32" s="2">
-        <v>45448.75138888889</v>
+        <v>45449.71736111111</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1678,16 +1648,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>100070</v>
+        <v>100054</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="2">
-        <v>45448.1875</v>
+        <v>45449.31041666667</v>
       </c>
       <c r="E33" s="2">
-        <v>45448.520875</v>
+        <v>45449.59861111111</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1695,16 +1665,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>100074</v>
+        <v>100060</v>
       </c>
       <c r="C34" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="2">
-        <v>45448.6875</v>
+        <v>45449.66666666666</v>
       </c>
       <c r="E34" s="2">
-        <v>45449.06386111111</v>
+        <v>45450.01858333333</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1712,16 +1682,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>100077</v>
+        <v>100061</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
       </c>
       <c r="D35" s="2">
-        <v>45448.25</v>
+        <v>45449.34444444445</v>
       </c>
       <c r="E35" s="2">
-        <v>45448.60094444444</v>
+        <v>45449.71138888889</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1729,16 +1699,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>100092</v>
+        <v>100068</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
       </c>
       <c r="D36" s="2">
-        <v>45448.69166666667</v>
+        <v>45449.54166666666</v>
       </c>
       <c r="E36" s="2">
-        <v>45448.93997222222</v>
+        <v>45449.95833333334</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1746,16 +1716,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>100134</v>
+        <v>100074</v>
       </c>
       <c r="C37" t="s">
         <v>39</v>
       </c>
       <c r="D37" s="2">
-        <v>45448.30277777778</v>
+        <v>45448.6875</v>
       </c>
       <c r="E37" s="2">
-        <v>45448.60416666666</v>
+        <v>45449.06386111111</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1763,16 +1733,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>100142</v>
+        <v>100076</v>
       </c>
       <c r="C38" t="s">
         <v>40</v>
       </c>
       <c r="D38" s="2">
-        <v>45448.44861111111</v>
+        <v>45449.66666666666</v>
       </c>
       <c r="E38" s="2">
-        <v>45448.72880555555</v>
+        <v>45450.03886111111</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1780,16 +1750,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>100261</v>
+        <v>100091</v>
       </c>
       <c r="C39" t="s">
         <v>41</v>
       </c>
       <c r="D39" s="2">
-        <v>45448.33263888889</v>
+        <v>45449.66666666666</v>
       </c>
       <c r="E39" s="2">
-        <v>45448.62361111111</v>
+        <v>45450.02777777778</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1797,16 +1767,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>100262</v>
+        <v>100092</v>
       </c>
       <c r="C40" t="s">
         <v>42</v>
       </c>
       <c r="D40" s="2">
-        <v>45448.41597222222</v>
+        <v>45448.69166666667</v>
       </c>
       <c r="E40" s="2">
-        <v>45448.70694444444</v>
+        <v>45448.93997222222</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1814,16 +1784,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>100263</v>
+        <v>100097</v>
       </c>
       <c r="C41" t="s">
         <v>43</v>
       </c>
       <c r="D41" s="2">
-        <v>45448.37430555555</v>
+        <v>45449.28263888889</v>
       </c>
       <c r="E41" s="2">
-        <v>45448.66527777778</v>
+        <v>45449.425</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1831,16 +1801,16 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>100264</v>
+        <v>100115</v>
       </c>
       <c r="C42" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="2">
-        <v>45448.29097222222</v>
+        <v>45449.35416666666</v>
       </c>
       <c r="E42" s="2">
-        <v>45448.58194444444</v>
+        <v>45449.63668055556</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1848,16 +1818,16 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>100284</v>
+        <v>100127</v>
       </c>
       <c r="C43" t="s">
         <v>45</v>
       </c>
       <c r="D43" s="2">
-        <v>45448.41666666666</v>
+        <v>45449.30277777778</v>
       </c>
       <c r="E43" s="2">
-        <v>45448.80277777778</v>
+        <v>45449.60833333333</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1865,16 +1835,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>100289</v>
+        <v>100135</v>
       </c>
       <c r="C44" t="s">
         <v>46</v>
       </c>
       <c r="D44" s="2">
-        <v>45448.27083333334</v>
+        <v>45449.30277777778</v>
       </c>
       <c r="E44" s="2">
-        <v>45448.65694444445</v>
+        <v>45449.60416666666</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1882,16 +1852,16 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>100326</v>
+        <v>100277</v>
       </c>
       <c r="C45" t="s">
         <v>47</v>
       </c>
       <c r="D45" s="2">
-        <v>45448.35416666666</v>
+        <v>45449.43888888889</v>
       </c>
       <c r="E45" s="2">
-        <v>45448.74027777778</v>
+        <v>45449.49444444444</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1899,16 +1869,16 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>100327</v>
+        <v>100278</v>
       </c>
       <c r="C46" t="s">
         <v>48</v>
       </c>
       <c r="D46" s="2">
-        <v>45448.27708333333</v>
+        <v>45448.81666666667</v>
       </c>
       <c r="E46" s="2">
-        <v>45448.44130555556</v>
+        <v>45448.87222222222</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1916,16 +1886,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>100331</v>
+        <v>100285</v>
       </c>
       <c r="C47" t="s">
         <v>49</v>
       </c>
       <c r="D47" s="2">
-        <v>45448.40208333333</v>
+        <v>45449.35416666666</v>
       </c>
       <c r="E47" s="2">
-        <v>45448.68783333333</v>
+        <v>45449.74027777778</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1933,16 +1903,16 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>100335</v>
+        <v>100288</v>
       </c>
       <c r="C48" t="s">
         <v>50</v>
       </c>
       <c r="D48" s="2">
-        <v>45448.31875</v>
+        <v>45449.27083333334</v>
       </c>
       <c r="E48" s="2">
-        <v>45448.6045</v>
+        <v>45449.65694444445</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1950,16 +1920,16 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>100341</v>
+        <v>100290</v>
       </c>
       <c r="C49" t="s">
         <v>51</v>
       </c>
       <c r="D49" s="2">
-        <v>45448.55555555555</v>
+        <v>45449.41666666666</v>
       </c>
       <c r="E49" s="2">
-        <v>45448.61111111111</v>
+        <v>45449.80277777778</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1967,16 +1937,16 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>100362</v>
+        <v>100329</v>
       </c>
       <c r="C50" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="2">
-        <v>45448.89583333334</v>
+        <v>45449.40208333333</v>
       </c>
       <c r="E50" s="2">
-        <v>45448.95138888889</v>
+        <v>45449.56630555556</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1984,16 +1954,16 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>100363</v>
+        <v>100332</v>
       </c>
       <c r="C51" t="s">
         <v>53</v>
       </c>
       <c r="D51" s="2">
-        <v>45448.26388888889</v>
+        <v>45449.40694444445</v>
       </c>
       <c r="E51" s="2">
-        <v>45448.61636111111</v>
+        <v>45449.56630555556</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2001,16 +1971,16 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>100364</v>
+        <v>100343</v>
       </c>
       <c r="C52" t="s">
         <v>54</v>
       </c>
       <c r="D52" s="2">
-        <v>45448.64236111111</v>
+        <v>45449.66666666666</v>
       </c>
       <c r="E52" s="2">
-        <v>45448.69791666666</v>
+        <v>45450.02777777778</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2018,16 +1988,16 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>100373</v>
+        <v>100351</v>
       </c>
       <c r="C53" t="s">
         <v>55</v>
       </c>
       <c r="D53" s="2">
-        <v>45448.27083333334</v>
+        <v>45449.31875</v>
       </c>
       <c r="E53" s="2">
-        <v>45448.61202777778</v>
+        <v>45449.48297222222</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2035,16 +2005,16 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>100379</v>
+        <v>100356</v>
       </c>
       <c r="C54" t="s">
         <v>56</v>
       </c>
       <c r="D54" s="2">
-        <v>45448.29166666666</v>
+        <v>45449.29166666666</v>
       </c>
       <c r="E54" s="2">
-        <v>45448.67430555556</v>
+        <v>45449.55138888889</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2052,16 +2022,16 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>100382</v>
+        <v>100362</v>
       </c>
       <c r="C55" t="s">
         <v>57</v>
       </c>
       <c r="D55" s="2">
-        <v>45448.29166666666</v>
+        <v>45448.89583333334</v>
       </c>
       <c r="E55" s="2">
-        <v>45448.48297222222</v>
+        <v>45449.61636111111</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2069,16 +2039,16 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>100386</v>
+        <v>100390</v>
       </c>
       <c r="C56" t="s">
         <v>58</v>
       </c>
       <c r="D56" s="2">
-        <v>45448.375</v>
+        <v>45449.5</v>
       </c>
       <c r="E56" s="2">
-        <v>45448.70486111111</v>
+        <v>45449.69130555556</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2086,16 +2056,16 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>100388</v>
+        <v>100401</v>
       </c>
       <c r="C57" t="s">
         <v>59</v>
       </c>
       <c r="D57" s="2">
-        <v>45448.29166666666</v>
+        <v>45449.29861111111</v>
       </c>
       <c r="E57" s="2">
-        <v>45448.62152777778</v>
+        <v>45449.60277777778</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2120,16 +2090,16 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>100417</v>
+        <v>100406</v>
       </c>
       <c r="C59" t="s">
         <v>61</v>
       </c>
       <c r="D59" s="2">
-        <v>45448.54861111111</v>
+        <v>45449.39444444444</v>
       </c>
       <c r="E59" s="2">
-        <v>45448.89691666666</v>
+        <v>45449.74027777778</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2137,16 +2107,16 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>100421</v>
+        <v>100408</v>
       </c>
       <c r="C60" t="s">
         <v>62</v>
       </c>
       <c r="D60" s="2">
-        <v>45448.69930555556</v>
+        <v>45449.70833333334</v>
       </c>
       <c r="E60" s="2">
-        <v>45449.02897222222</v>
+        <v>45450.09305555555</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2154,16 +2124,16 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>100434</v>
+        <v>100409</v>
       </c>
       <c r="C61" t="s">
         <v>63</v>
       </c>
       <c r="D61" s="2">
-        <v>45448.52083333334</v>
+        <v>45449.39583333334</v>
       </c>
       <c r="E61" s="2">
-        <v>45448.9375</v>
+        <v>45449.72430555556</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2171,16 +2141,16 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>100442</v>
+        <v>100420</v>
       </c>
       <c r="C62" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="2">
-        <v>45448.61180555556</v>
+        <v>45449.61388888889</v>
       </c>
       <c r="E62" s="2">
-        <v>45448.95233333333</v>
+        <v>45449.9125</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2188,16 +2158,16 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>100444</v>
+        <v>100421</v>
       </c>
       <c r="C63" t="s">
         <v>65</v>
       </c>
       <c r="D63" s="2">
-        <v>45448.7375</v>
+        <v>45448.69930555556</v>
       </c>
       <c r="E63" s="2">
-        <v>45449.05140277778</v>
+        <v>45449.02897222222</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2205,16 +2175,16 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>100465</v>
+        <v>100422</v>
       </c>
       <c r="C64" t="s">
         <v>66</v>
       </c>
       <c r="D64" s="2">
-        <v>45448.69236111111</v>
+        <v>45449.39444444444</v>
       </c>
       <c r="E64" s="2">
-        <v>45449.08333333334</v>
+        <v>45449.66597222222</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2222,16 +2192,16 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>100477</v>
+        <v>100423</v>
       </c>
       <c r="C65" t="s">
         <v>67</v>
       </c>
       <c r="D65" s="2">
-        <v>45448.70833333334</v>
+        <v>45449.77083333334</v>
       </c>
       <c r="E65" s="2">
-        <v>45449.02152777778</v>
+        <v>45450.15416666667</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2239,16 +2209,16 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>100479</v>
+        <v>100425</v>
       </c>
       <c r="C66" t="s">
         <v>68</v>
       </c>
       <c r="D66" s="2">
-        <v>45448.70833333334</v>
+        <v>45449.25</v>
       </c>
       <c r="E66" s="2">
-        <v>45449.17876388889</v>
+        <v>45449.66666666666</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2256,16 +2226,16 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>100490</v>
+        <v>100441</v>
       </c>
       <c r="C67" t="s">
         <v>69</v>
       </c>
       <c r="D67" s="2">
-        <v>45448.61597222222</v>
+        <v>45449.66666666666</v>
       </c>
       <c r="E67" s="2">
-        <v>45448.75833333333</v>
+        <v>45450.05569444445</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2273,16 +2243,16 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>100496</v>
+        <v>100444</v>
       </c>
       <c r="C68" t="s">
         <v>70</v>
       </c>
       <c r="D68" s="2">
-        <v>45448.39583333334</v>
+        <v>45448.7375</v>
       </c>
       <c r="E68" s="2">
-        <v>45448.72361111111</v>
+        <v>45449.05140277778</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2290,16 +2260,16 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>100511</v>
+        <v>100456</v>
       </c>
       <c r="C69" t="s">
         <v>71</v>
       </c>
       <c r="D69" s="2">
-        <v>45448.70833333334</v>
+        <v>45449.64583333334</v>
       </c>
       <c r="E69" s="2">
-        <v>45449.07955555555</v>
+        <v>45449.96204166667</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2307,16 +2277,16 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>100530</v>
+        <v>100465</v>
       </c>
       <c r="C70" t="s">
         <v>72</v>
       </c>
       <c r="D70" s="2">
-        <v>45448.20833333334</v>
+        <v>45448.69236111111</v>
       </c>
       <c r="E70" s="2">
-        <v>45448.53611111111</v>
+        <v>45449.08333333334</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2324,16 +2294,16 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>100540</v>
+        <v>100467</v>
       </c>
       <c r="C71" t="s">
         <v>73</v>
       </c>
       <c r="D71" s="2">
-        <v>45448.41944444444</v>
+        <v>45449.69375</v>
       </c>
       <c r="E71" s="2">
-        <v>45448.475</v>
+        <v>45450.01594444444</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2341,16 +2311,16 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>100541</v>
+        <v>100475</v>
       </c>
       <c r="C72" t="s">
         <v>74</v>
       </c>
       <c r="D72" s="2">
-        <v>45448.69444444445</v>
+        <v>45449.27083333334</v>
       </c>
       <c r="E72" s="2">
-        <v>45448.75</v>
+        <v>45449.59930555556</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2358,16 +2328,16 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>100542</v>
+        <v>100477</v>
       </c>
       <c r="C73" t="s">
         <v>75</v>
       </c>
       <c r="D73" s="2">
-        <v>45448.69444444445</v>
+        <v>45448.70833333334</v>
       </c>
       <c r="E73" s="2">
-        <v>45448.75</v>
+        <v>45449.02152777778</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2375,16 +2345,16 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>100543</v>
+        <v>100479</v>
       </c>
       <c r="C74" t="s">
         <v>76</v>
       </c>
       <c r="D74" s="2">
-        <v>45448.73472222222</v>
+        <v>45448.70833333334</v>
       </c>
       <c r="E74" s="2">
-        <v>45448.79027777778</v>
+        <v>45449.17876388889</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2392,16 +2362,16 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>100553</v>
+        <v>100484</v>
       </c>
       <c r="C75" t="s">
         <v>77</v>
       </c>
       <c r="D75" s="2">
-        <v>45448.69583333333</v>
+        <v>45449.7125</v>
       </c>
       <c r="E75" s="2">
-        <v>45448.75138888889</v>
+        <v>45450.08655555556</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2409,16 +2379,16 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>100554</v>
+        <v>100490</v>
       </c>
       <c r="C76" t="s">
         <v>78</v>
       </c>
       <c r="D76" s="2">
-        <v>45448.8375</v>
+        <v>45448.67847222222</v>
       </c>
       <c r="E76" s="2">
-        <v>45448.89305555556</v>
+        <v>45448.82083333333</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2426,16 +2396,16 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>100556</v>
+        <v>100503</v>
       </c>
       <c r="C77" t="s">
         <v>79</v>
       </c>
       <c r="D77" s="2">
-        <v>45448.35416666666</v>
+        <v>45449.66666666666</v>
       </c>
       <c r="E77" s="2">
-        <v>45448.66491666667</v>
+        <v>45449.94644444445</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2443,16 +2413,16 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>100590</v>
+        <v>100511</v>
       </c>
       <c r="C78" t="s">
         <v>80</v>
       </c>
       <c r="D78" s="2">
-        <v>45448.75833333333</v>
+        <v>45449.70833333334</v>
       </c>
       <c r="E78" s="2">
-        <v>45448.81388888889</v>
+        <v>45450.07955555555</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2460,16 +2430,16 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>100603</v>
+        <v>100541</v>
       </c>
       <c r="C79" t="s">
         <v>81</v>
       </c>
       <c r="D79" s="2">
-        <v>45448.29583333333</v>
+        <v>45448.725</v>
       </c>
       <c r="E79" s="2">
-        <v>45448.63263888889</v>
+        <v>45448.78055555555</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2477,16 +2447,16 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>100604</v>
+        <v>100542</v>
       </c>
       <c r="C80" t="s">
         <v>82</v>
       </c>
       <c r="D80" s="2">
-        <v>45448.46944444445</v>
+        <v>45448.69444444445</v>
       </c>
       <c r="E80" s="2">
-        <v>45448.525</v>
+        <v>45448.75</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2494,16 +2464,16 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>100610</v>
+        <v>100543</v>
       </c>
       <c r="C81" t="s">
         <v>83</v>
       </c>
       <c r="D81" s="2">
-        <v>45448.41527777778</v>
+        <v>45448.73472222222</v>
       </c>
       <c r="E81" s="2">
-        <v>45448.47083333333</v>
+        <v>45448.79027777778</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2511,16 +2481,16 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>100611</v>
+        <v>100546</v>
       </c>
       <c r="C82" t="s">
         <v>84</v>
       </c>
       <c r="D82" s="2">
-        <v>45448.43611111111</v>
+        <v>45449.56111111111</v>
       </c>
       <c r="E82" s="2">
-        <v>45448.49166666667</v>
+        <v>45449.61666666667</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2528,16 +2498,16 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>100612</v>
+        <v>100553</v>
       </c>
       <c r="C83" t="s">
         <v>85</v>
       </c>
       <c r="D83" s="2">
-        <v>45448.41388888889</v>
+        <v>45448.69583333333</v>
       </c>
       <c r="E83" s="2">
-        <v>45448.46944444445</v>
+        <v>45449.61908333333</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2545,16 +2515,16 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>100613</v>
+        <v>100554</v>
       </c>
       <c r="C84" t="s">
         <v>86</v>
       </c>
       <c r="D84" s="2">
-        <v>45448.54722222222</v>
+        <v>45448.8375</v>
       </c>
       <c r="E84" s="2">
-        <v>45448.60277777778</v>
+        <v>45449.77533333333</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2562,16 +2532,16 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>100614</v>
+        <v>100590</v>
       </c>
       <c r="C85" t="s">
         <v>87</v>
       </c>
       <c r="D85" s="2">
-        <v>45448.32916666667</v>
+        <v>45448.75833333333</v>
       </c>
       <c r="E85" s="2">
-        <v>45448.38472222222</v>
+        <v>45449.66483333334</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2579,16 +2549,16 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>100615</v>
+        <v>100604</v>
       </c>
       <c r="C86" t="s">
         <v>88</v>
       </c>
       <c r="D86" s="2">
-        <v>45448.52708333333</v>
+        <v>45449.27013888889</v>
       </c>
       <c r="E86" s="2">
-        <v>45448.58263888889</v>
+        <v>45449.53844444444</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2596,16 +2566,16 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>100616</v>
+        <v>100605</v>
       </c>
       <c r="C87" t="s">
         <v>89</v>
       </c>
       <c r="D87" s="2">
-        <v>45448.41111111111</v>
+        <v>45448.72916666666</v>
       </c>
       <c r="E87" s="2">
-        <v>45448.46666666667</v>
+        <v>45448.78472222222</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2613,16 +2583,16 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>100617</v>
+        <v>100606</v>
       </c>
       <c r="C88" t="s">
         <v>90</v>
       </c>
       <c r="D88" s="2">
-        <v>45448.34236111111</v>
+        <v>45449.33888888889</v>
       </c>
       <c r="E88" s="2">
-        <v>45448.39791666667</v>
+        <v>45449.39444444444</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2630,16 +2600,16 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>100636</v>
+        <v>100614</v>
       </c>
       <c r="C89" t="s">
         <v>91</v>
       </c>
       <c r="D89" s="2">
-        <v>45448.55694444444</v>
+        <v>45449.72013888889</v>
       </c>
       <c r="E89" s="2">
-        <v>45448.6125</v>
+        <v>45450.00715277778</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2647,16 +2617,16 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>100642</v>
+        <v>100618</v>
       </c>
       <c r="C90" t="s">
         <v>92</v>
       </c>
       <c r="D90" s="2">
-        <v>45448.55486111111</v>
+        <v>45448.81666666667</v>
       </c>
       <c r="E90" s="2">
-        <v>45448.61041666667</v>
+        <v>45448.87222222222</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2664,16 +2634,16 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>100650</v>
+        <v>100619</v>
       </c>
       <c r="C91" t="s">
         <v>93</v>
       </c>
       <c r="D91" s="2">
-        <v>45448.16875</v>
+        <v>45448.84583333333</v>
       </c>
       <c r="E91" s="2">
-        <v>45448.22430555556</v>
+        <v>45448.90138888889</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2681,16 +2651,16 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>100651</v>
+        <v>100620</v>
       </c>
       <c r="C92" t="s">
         <v>94</v>
       </c>
       <c r="D92" s="2">
-        <v>45448.53680555556</v>
+        <v>45448.83333333334</v>
       </c>
       <c r="E92" s="2">
-        <v>45448.59236111111</v>
+        <v>45448.88888888889</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2698,16 +2668,16 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>100653</v>
+        <v>100621</v>
       </c>
       <c r="C93" t="s">
         <v>95</v>
       </c>
       <c r="D93" s="2">
-        <v>45448.44861111111</v>
+        <v>45448.68611111111</v>
       </c>
       <c r="E93" s="2">
-        <v>45448.50416666667</v>
+        <v>45448.74166666667</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2715,16 +2685,16 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>100654</v>
+        <v>100622</v>
       </c>
       <c r="C94" t="s">
         <v>96</v>
       </c>
       <c r="D94" s="2">
-        <v>45448.57361111111</v>
+        <v>45448.70972222222</v>
       </c>
       <c r="E94" s="2">
-        <v>45448.62916666667</v>
+        <v>45448.76527777778</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2732,16 +2702,16 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>100656</v>
+        <v>100623</v>
       </c>
       <c r="C95" t="s">
         <v>97</v>
       </c>
       <c r="D95" s="2">
-        <v>45448.51527777778</v>
+        <v>45448.68333333333</v>
       </c>
       <c r="E95" s="2">
-        <v>45448.57083333333</v>
+        <v>45448.73888888889</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2749,16 +2719,16 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>100658</v>
+        <v>100624</v>
       </c>
       <c r="C96" t="s">
         <v>98</v>
       </c>
       <c r="D96" s="2">
-        <v>45448.725</v>
+        <v>45448.88055555556</v>
       </c>
       <c r="E96" s="2">
-        <v>45448.78055555555</v>
+        <v>45448.93611111111</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2766,16 +2736,16 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>100660</v>
+        <v>100625</v>
       </c>
       <c r="C97" t="s">
         <v>99</v>
       </c>
       <c r="D97" s="2">
-        <v>45448.64583333334</v>
+        <v>45448.7125</v>
       </c>
       <c r="E97" s="2">
-        <v>45448.70138888889</v>
+        <v>45448.76805555556</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2783,16 +2753,16 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>100661</v>
+        <v>100628</v>
       </c>
       <c r="C98" t="s">
         <v>100</v>
       </c>
       <c r="D98" s="2">
-        <v>45448.55694444444</v>
+        <v>45448.69583333333</v>
       </c>
       <c r="E98" s="2">
-        <v>45448.6125</v>
+        <v>45448.75138888889</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2800,16 +2770,16 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>100663</v>
+        <v>100629</v>
       </c>
       <c r="C99" t="s">
         <v>101</v>
       </c>
       <c r="D99" s="2">
-        <v>45448.74722222222</v>
+        <v>45448.73055555556</v>
       </c>
       <c r="E99" s="2">
-        <v>45448.80277777778</v>
+        <v>45448.78611111111</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2817,16 +2787,16 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>100667</v>
+        <v>100630</v>
       </c>
       <c r="C100" t="s">
         <v>102</v>
       </c>
       <c r="D100" s="2">
-        <v>45448.425</v>
+        <v>45449.52083333334</v>
       </c>
       <c r="E100" s="2">
-        <v>45448.48055555556</v>
+        <v>45449.57638888889</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2834,16 +2804,16 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>100669</v>
+        <v>100632</v>
       </c>
       <c r="C101" t="s">
         <v>103</v>
       </c>
       <c r="D101" s="2">
-        <v>45448.35416666666</v>
+        <v>45448.74027777778</v>
       </c>
       <c r="E101" s="2">
-        <v>45448.40972222222</v>
+        <v>45450.02777777778</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2851,16 +2821,16 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>100672</v>
+        <v>100643</v>
       </c>
       <c r="C102" t="s">
         <v>104</v>
       </c>
       <c r="D102" s="2">
-        <v>45448.37847222222</v>
+        <v>45449.37638888889</v>
       </c>
       <c r="E102" s="2">
-        <v>45448.43402777778</v>
+        <v>45449.43194444444</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2868,16 +2838,16 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>100673</v>
+        <v>100644</v>
       </c>
       <c r="C103" t="s">
         <v>105</v>
       </c>
       <c r="D103" s="2">
-        <v>45448.44722222222</v>
+        <v>45448.85277777778</v>
       </c>
       <c r="E103" s="2">
-        <v>45448.50277777778</v>
+        <v>45448.90833333333</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2885,16 +2855,16 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>100674</v>
+        <v>100645</v>
       </c>
       <c r="C104" t="s">
         <v>106</v>
       </c>
       <c r="D104" s="2">
-        <v>45448.72916666666</v>
+        <v>45448.69722222222</v>
       </c>
       <c r="E104" s="2">
-        <v>45448.78472222222</v>
+        <v>45448.75277777778</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2902,16 +2872,16 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>100678</v>
+        <v>100646</v>
       </c>
       <c r="C105" t="s">
         <v>107</v>
       </c>
       <c r="D105" s="2">
-        <v>45448.56388888889</v>
+        <v>45449.45833333334</v>
       </c>
       <c r="E105" s="2">
-        <v>45448.61944444444</v>
+        <v>45449.51388888889</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2919,16 +2889,16 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>100680</v>
+        <v>100654</v>
       </c>
       <c r="C106" t="s">
         <v>108</v>
       </c>
       <c r="D106" s="2">
-        <v>45448.73055555556</v>
+        <v>45448.725</v>
       </c>
       <c r="E106" s="2">
-        <v>45448.78611111111</v>
+        <v>45448.78055555555</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2936,16 +2906,16 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>100681</v>
+        <v>100656</v>
       </c>
       <c r="C107" t="s">
         <v>109</v>
       </c>
       <c r="D107" s="2">
-        <v>45448.74305555555</v>
+        <v>45449.33333333334</v>
       </c>
       <c r="E107" s="2">
-        <v>45448.79861111111</v>
+        <v>45449.641</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2953,16 +2923,16 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>100682</v>
+        <v>100660</v>
       </c>
       <c r="C108" t="s">
         <v>110</v>
       </c>
       <c r="D108" s="2">
-        <v>45448.50833333333</v>
+        <v>45448.74722222222</v>
       </c>
       <c r="E108" s="2">
-        <v>45448.56388888889</v>
+        <v>45448.80277777778</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2970,16 +2940,16 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>100684</v>
+        <v>100672</v>
       </c>
       <c r="C109" t="s">
         <v>111</v>
       </c>
       <c r="D109" s="2">
-        <v>45448.33611111111</v>
+        <v>45448.72916666666</v>
       </c>
       <c r="E109" s="2">
-        <v>45448.39166666667</v>
+        <v>45448.78472222222</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2987,16 +2957,16 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>100685</v>
+        <v>100674</v>
       </c>
       <c r="C110" t="s">
         <v>112</v>
       </c>
       <c r="D110" s="2">
-        <v>45448.38888888889</v>
+        <v>45448.73055555556</v>
       </c>
       <c r="E110" s="2">
-        <v>45448.44444444445</v>
+        <v>45448.78611111111</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -3004,16 +2974,16 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>100686</v>
+        <v>100678</v>
       </c>
       <c r="C111" t="s">
         <v>113</v>
       </c>
       <c r="D111" s="2">
-        <v>45448.58194444444</v>
+        <v>45448.74305555555</v>
       </c>
       <c r="E111" s="2">
-        <v>45448.6375</v>
+        <v>45448.79861111111</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -3021,16 +2991,16 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>100689</v>
+        <v>100710</v>
       </c>
       <c r="C112" t="s">
         <v>114</v>
       </c>
       <c r="D112" s="2">
-        <v>45448.39583333334</v>
+        <v>45448.72222222222</v>
       </c>
       <c r="E112" s="2">
-        <v>45448.45138888889</v>
+        <v>45448.77777777778</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -3038,16 +3008,16 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>100690</v>
+        <v>100736</v>
       </c>
       <c r="C113" t="s">
         <v>115</v>
       </c>
       <c r="D113" s="2">
-        <v>45448.41944444444</v>
+        <v>45448.71388888889</v>
       </c>
       <c r="E113" s="2">
-        <v>45448.475</v>
+        <v>45449.48233333333</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -3055,16 +3025,16 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>100695</v>
+        <v>100738</v>
       </c>
       <c r="C114" t="s">
         <v>116</v>
       </c>
       <c r="D114" s="2">
-        <v>45448.45208333333</v>
+        <v>45449.28888888889</v>
       </c>
       <c r="E114" s="2">
-        <v>45448.50763888889</v>
+        <v>45449.48233333333</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3072,16 +3042,16 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>100696</v>
+        <v>100739</v>
       </c>
       <c r="C115" t="s">
         <v>117</v>
       </c>
       <c r="D115" s="2">
-        <v>45448.375</v>
+        <v>45449.28888888889</v>
       </c>
       <c r="E115" s="2">
-        <v>45448.43055555555</v>
+        <v>45449.48233333333</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3089,16 +3059,16 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>100702</v>
+        <v>100740</v>
       </c>
       <c r="C116" t="s">
         <v>118</v>
       </c>
       <c r="D116" s="2">
-        <v>45448.55416666667</v>
+        <v>45448.84930555556</v>
       </c>
       <c r="E116" s="2">
-        <v>45448.60972222222</v>
+        <v>45449.62361111111</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3106,16 +3076,16 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>100706</v>
+        <v>100741</v>
       </c>
       <c r="C117" t="s">
         <v>119</v>
       </c>
       <c r="D117" s="2">
-        <v>45448.5375</v>
+        <v>45449.35555555556</v>
       </c>
       <c r="E117" s="2">
-        <v>45448.59305555555</v>
+        <v>45449.41111111111</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3123,16 +3093,16 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>100707</v>
+        <v>100749</v>
       </c>
       <c r="C118" t="s">
         <v>120</v>
       </c>
       <c r="D118" s="2">
-        <v>45448.38055555556</v>
+        <v>45449.575</v>
       </c>
       <c r="E118" s="2">
-        <v>45448.43611111111</v>
+        <v>45449.63055555556</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3140,16 +3110,16 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>100710</v>
+        <v>100750</v>
       </c>
       <c r="C119" t="s">
         <v>121</v>
       </c>
       <c r="D119" s="2">
-        <v>45448.55138888889</v>
+        <v>45449.41944444444</v>
       </c>
       <c r="E119" s="2">
-        <v>45448.60694444444</v>
+        <v>45449.80380555556</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3157,16 +3127,16 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>100728</v>
+        <v>100752</v>
       </c>
       <c r="C120" t="s">
         <v>122</v>
       </c>
       <c r="D120" s="2">
-        <v>45448.42222222222</v>
+        <v>45449.42083333333</v>
       </c>
       <c r="E120" s="2">
-        <v>45448.47777777778</v>
+        <v>45449.80380555556</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3174,16 +3144,16 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>100729</v>
+        <v>100753</v>
       </c>
       <c r="C121" t="s">
         <v>123</v>
       </c>
       <c r="D121" s="2">
-        <v>45448.5625</v>
+        <v>45449.30972222222</v>
       </c>
       <c r="E121" s="2">
-        <v>45448.61805555555</v>
+        <v>45449.60980555556</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3191,16 +3161,16 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>100734</v>
+        <v>100776</v>
       </c>
       <c r="C122" t="s">
         <v>124</v>
       </c>
       <c r="D122" s="2">
-        <v>45448.72222222222</v>
+        <v>45448.84861111111</v>
       </c>
       <c r="E122" s="2">
-        <v>45448.77777777778</v>
+        <v>45448.90416666667</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3208,16 +3178,16 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>100736</v>
+        <v>100777</v>
       </c>
       <c r="C123" t="s">
         <v>125</v>
       </c>
       <c r="D123" s="2">
-        <v>45448.32361111111</v>
+        <v>45448.89305555556</v>
       </c>
       <c r="E123" s="2">
-        <v>45448.47916666666</v>
+        <v>45448.94861111111</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3225,16 +3195,16 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>100738</v>
+        <v>100782</v>
       </c>
       <c r="C124" t="s">
         <v>126</v>
       </c>
       <c r="D124" s="2">
-        <v>45448.45902777778</v>
+        <v>45448.69305555556</v>
       </c>
       <c r="E124" s="2">
-        <v>45448.61458333334</v>
+        <v>45448.77638888889</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3242,16 +3212,16 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>100739</v>
+        <v>100800</v>
       </c>
       <c r="C125" t="s">
         <v>127</v>
       </c>
       <c r="D125" s="2">
-        <v>45448.58333333334</v>
+        <v>45448.74444444444</v>
       </c>
       <c r="E125" s="2">
-        <v>45448.79166666666</v>
+        <v>45449.61202777778</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3259,16 +3229,16 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>100740</v>
+        <v>100801</v>
       </c>
       <c r="C126" t="s">
         <v>128</v>
       </c>
       <c r="D126" s="2">
-        <v>45448.71388888889</v>
+        <v>45449.57222222222</v>
       </c>
       <c r="E126" s="2">
-        <v>45448.76944444444</v>
+        <v>45449.87083333333</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3276,16 +3246,16 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>100753</v>
+        <v>100804</v>
       </c>
       <c r="C127" t="s">
         <v>129</v>
       </c>
       <c r="D127" s="2">
-        <v>45448.55833333333</v>
+        <v>45449.70833333334</v>
       </c>
       <c r="E127" s="2">
-        <v>45448.61388888889</v>
+        <v>45449.91666666666</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3293,16 +3263,16 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>100766</v>
+        <v>100821</v>
       </c>
       <c r="C128" t="s">
         <v>130</v>
       </c>
       <c r="D128" s="2">
-        <v>45448.55694444444</v>
+        <v>45449.27083333334</v>
       </c>
       <c r="E128" s="2">
-        <v>45448.6125</v>
+        <v>45449.71805555555</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3310,16 +3280,16 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>100767</v>
+        <v>100860</v>
       </c>
       <c r="C129" t="s">
         <v>131</v>
       </c>
       <c r="D129" s="2">
-        <v>45448.84930555556</v>
+        <v>45449.47222222222</v>
       </c>
       <c r="E129" s="2">
-        <v>45448.90486111111</v>
+        <v>45449.52777777778</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3327,16 +3297,16 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>100768</v>
+        <v>100862</v>
       </c>
       <c r="C130" t="s">
         <v>132</v>
       </c>
       <c r="D130" s="2">
-        <v>45448.65277777778</v>
+        <v>45449.53472222222</v>
       </c>
       <c r="E130" s="2">
-        <v>45448.70833333334</v>
+        <v>45449.59027777778</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3344,16 +3314,16 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>100770</v>
+        <v>100904</v>
       </c>
       <c r="C131" t="s">
         <v>133</v>
       </c>
       <c r="D131" s="2">
-        <v>45448.44236111111</v>
+        <v>45449.54166666666</v>
       </c>
       <c r="E131" s="2">
-        <v>45448.49791666667</v>
+        <v>45449.75</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3361,356 +3331,16 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>100771</v>
+        <v>100905</v>
       </c>
       <c r="C132" t="s">
         <v>134</v>
       </c>
       <c r="D132" s="2">
-        <v>45448.39722222222</v>
+        <v>45448.70555555556</v>
       </c>
       <c r="E132" s="2">
-        <v>45448.45277777778</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="1">
-        <v>131</v>
-      </c>
-      <c r="B133">
-        <v>100772</v>
-      </c>
-      <c r="C133" t="s">
-        <v>135</v>
-      </c>
-      <c r="D133" s="2">
-        <v>45448.37847222222</v>
-      </c>
-      <c r="E133" s="2">
-        <v>45448.43402777778</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="1">
-        <v>132</v>
-      </c>
-      <c r="B134">
-        <v>100773</v>
-      </c>
-      <c r="C134" t="s">
-        <v>136</v>
-      </c>
-      <c r="D134" s="2">
-        <v>45448.36666666667</v>
-      </c>
-      <c r="E134" s="2">
-        <v>45448.42222222222</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
-      <c r="A135" s="1">
-        <v>133</v>
-      </c>
-      <c r="B135">
-        <v>100774</v>
-      </c>
-      <c r="C135" t="s">
-        <v>137</v>
-      </c>
-      <c r="D135" s="2">
-        <v>45448.39513888889</v>
-      </c>
-      <c r="E135" s="2">
-        <v>45448.45069444444</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="1">
-        <v>134</v>
-      </c>
-      <c r="B136">
-        <v>100775</v>
-      </c>
-      <c r="C136" t="s">
-        <v>138</v>
-      </c>
-      <c r="D136" s="2">
-        <v>45448.35138888889</v>
-      </c>
-      <c r="E136" s="2">
-        <v>45448.40694444445</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="1">
-        <v>135</v>
-      </c>
-      <c r="B137">
-        <v>100778</v>
-      </c>
-      <c r="C137" t="s">
-        <v>139</v>
-      </c>
-      <c r="D137" s="2">
-        <v>45448.43194444444</v>
-      </c>
-      <c r="E137" s="2">
-        <v>45448.4875</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
-      <c r="A138" s="1">
-        <v>136</v>
-      </c>
-      <c r="B138">
-        <v>100782</v>
-      </c>
-      <c r="C138" t="s">
-        <v>140</v>
-      </c>
-      <c r="D138" s="2">
-        <v>45448.33194444444</v>
-      </c>
-      <c r="E138" s="2">
-        <v>45448.3875</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="1">
-        <v>137</v>
-      </c>
-      <c r="B139">
-        <v>100794</v>
-      </c>
-      <c r="C139" t="s">
-        <v>141</v>
-      </c>
-      <c r="D139" s="2">
-        <v>45448.44027777778</v>
-      </c>
-      <c r="E139" s="2">
-        <v>45448.49583333333</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="1">
-        <v>138</v>
-      </c>
-      <c r="B140">
-        <v>100795</v>
-      </c>
-      <c r="C140" t="s">
-        <v>142</v>
-      </c>
-      <c r="D140" s="2">
-        <v>45448.53541666667</v>
-      </c>
-      <c r="E140" s="2">
-        <v>45448.59097222222</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
-      <c r="A141" s="1">
-        <v>139</v>
-      </c>
-      <c r="B141">
-        <v>100796</v>
-      </c>
-      <c r="C141" t="s">
-        <v>143</v>
-      </c>
-      <c r="D141" s="2">
-        <v>45448.69305555556</v>
-      </c>
-      <c r="E141" s="2">
-        <v>45448.77638888889</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
-      <c r="A142" s="1">
-        <v>140</v>
-      </c>
-      <c r="B142">
-        <v>100797</v>
-      </c>
-      <c r="C142" t="s">
-        <v>144</v>
-      </c>
-      <c r="D142" s="2">
-        <v>45448.43472222222</v>
-      </c>
-      <c r="E142" s="2">
-        <v>45448.49027777778</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="A143" s="1">
-        <v>141</v>
-      </c>
-      <c r="B143">
-        <v>100801</v>
-      </c>
-      <c r="C143" t="s">
-        <v>145</v>
-      </c>
-      <c r="D143" s="2">
-        <v>45448.40694444445</v>
-      </c>
-      <c r="E143" s="2">
-        <v>45448.4625</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="A144" s="1">
-        <v>142</v>
-      </c>
-      <c r="B144">
-        <v>100802</v>
-      </c>
-      <c r="C144" t="s">
-        <v>146</v>
-      </c>
-      <c r="D144" s="2">
-        <v>45448.44444444445</v>
-      </c>
-      <c r="E144" s="2">
-        <v>45448.5</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5">
-      <c r="A145" s="1">
-        <v>143</v>
-      </c>
-      <c r="B145">
-        <v>100803</v>
-      </c>
-      <c r="C145" t="s">
-        <v>147</v>
-      </c>
-      <c r="D145" s="2">
-        <v>45448.45694444444</v>
-      </c>
-      <c r="E145" s="2">
-        <v>45448.5125</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
-      <c r="A146" s="1">
-        <v>144</v>
-      </c>
-      <c r="B146">
-        <v>100804</v>
-      </c>
-      <c r="C146" t="s">
-        <v>148</v>
-      </c>
-      <c r="D146" s="2">
-        <v>45448.66319444445</v>
-      </c>
-      <c r="E146" s="2">
-        <v>45448.71875</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="1">
-        <v>145</v>
-      </c>
-      <c r="B147">
-        <v>100805</v>
-      </c>
-      <c r="C147" t="s">
-        <v>149</v>
-      </c>
-      <c r="D147" s="2">
-        <v>45448.67013888889</v>
-      </c>
-      <c r="E147" s="2">
-        <v>45448.72569444445</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
-      <c r="A148" s="1">
-        <v>146</v>
-      </c>
-      <c r="B148">
-        <v>100821</v>
-      </c>
-      <c r="C148" t="s">
-        <v>150</v>
-      </c>
-      <c r="D148" s="2">
-        <v>45448.55555555555</v>
-      </c>
-      <c r="E148" s="2">
-        <v>45448.61111111111</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
-      <c r="A149" s="1">
-        <v>147</v>
-      </c>
-      <c r="B149">
-        <v>100807</v>
-      </c>
-      <c r="C149" t="s">
-        <v>151</v>
-      </c>
-      <c r="D149" s="2">
-        <v>45448.375</v>
-      </c>
-      <c r="E149" s="2">
-        <v>45448.48611111111</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
-      <c r="A150" s="1">
-        <v>148</v>
-      </c>
-      <c r="B150">
-        <v>100640</v>
-      </c>
-      <c r="C150" t="s">
-        <v>152</v>
-      </c>
-      <c r="D150" s="2">
-        <v>45448.56388888889</v>
-      </c>
-      <c r="E150" s="2">
-        <v>45448.61944444444</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
-      <c r="A151" s="1">
-        <v>149</v>
-      </c>
-      <c r="B151">
-        <v>100631</v>
-      </c>
-      <c r="C151" t="s">
-        <v>153</v>
-      </c>
-      <c r="D151" s="2">
-        <v>45448.38611111111</v>
-      </c>
-      <c r="E151" s="2">
-        <v>45448.44166666667</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
-      <c r="A152" s="1">
-        <v>150</v>
-      </c>
-      <c r="B152">
-        <v>100703</v>
-      </c>
-      <c r="C152" t="s">
-        <v>154</v>
-      </c>
-      <c r="D152" s="2">
-        <v>45448.56111111111</v>
-      </c>
-      <c r="E152" s="2">
-        <v>45448.61666666667</v>
+        <v>45449.56944444445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>